<commit_message>
updated getting urls from xlsx, fixed scraping stats
</commit_message>
<xml_diff>
--- a/urls.xlsx
+++ b/urls.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maciek\Desktop\python_projects\flashscore_scraper\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maciej\Desktop\python_projects\flashscore-scraper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8029955-20E8-4785-B0E4-05DE2707D430}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{207B4998-54A4-4C0E-B411-49E67B1F2ECE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -30,12 +30,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="12">
   <si>
     <t>URL</t>
-  </si>
-  <si>
-    <t>Done</t>
   </si>
   <si>
     <t>year1</t>
@@ -489,27 +486,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G252"/>
+  <dimension ref="A1:F252"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="C1" sqref="C1:C1048576"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="77.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="67.85546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="77.88671875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="67.88671875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" t="s">
+        <v>5</v>
+      </c>
+      <c r="D1" t="s">
         <v>1</v>
-      </c>
-      <c r="D1" t="s">
-        <v>6</v>
       </c>
       <c r="E1" t="s">
         <v>2</v>
@@ -517,50 +514,47 @@
       <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="G1" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>0</v>
       </c>
       <c r="B2" s="2" t="str">
-        <f>D2&amp;E2&amp;F2&amp;$G$2</f>
+        <f>C2&amp;D2&amp;E2&amp;$F$2</f>
         <v>https://www.flashscore.com/football/czech-republic/1-liga-2019-2020/results/</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>7</v>
+      <c r="C2" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D2">
+        <v>-2019</v>
       </c>
       <c r="E2">
-        <v>-2019</v>
-      </c>
-      <c r="F2">
         <v>-2020</v>
       </c>
-      <c r="G2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F2" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
       <c r="B3" s="2" t="str">
-        <f t="shared" ref="B3:B21" si="0">D3&amp;E3&amp;F3&amp;$G$2</f>
+        <f t="shared" ref="B3:B21" si="0">C3&amp;D3&amp;E3&amp;$F$2</f>
         <v>https://www.flashscore.com/football/czech-republic/1-liga-2018-2019/results/</v>
       </c>
-      <c r="D3" s="2" t="s">
-        <v>7</v>
+      <c r="C3" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D3">
+        <v>-2018</v>
       </c>
       <c r="E3">
-        <v>-2018</v>
-      </c>
-      <c r="F3">
         <v>-2019</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -568,17 +562,17 @@
         <f t="shared" si="0"/>
         <v>https://www.flashscore.com/football/czech-republic/1-liga-2017-2018/results/</v>
       </c>
-      <c r="D4" s="2" t="s">
-        <v>7</v>
+      <c r="C4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D4">
+        <v>-2017</v>
       </c>
       <c r="E4">
-        <v>-2017</v>
-      </c>
-      <c r="F4">
         <v>-2018</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -586,17 +580,17 @@
         <f t="shared" si="0"/>
         <v>https://www.flashscore.com/football/czech-republic/1-liga-2016-2017/results/</v>
       </c>
-      <c r="D5" s="2" t="s">
-        <v>7</v>
+      <c r="C5" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D5">
+        <v>-2016</v>
       </c>
       <c r="E5">
-        <v>-2016</v>
-      </c>
-      <c r="F5">
         <v>-2017</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -604,17 +598,17 @@
         <f t="shared" si="0"/>
         <v>https://www.flashscore.com/football/czech-republic/1-liga-2015-2016/results/</v>
       </c>
-      <c r="D6" s="2" t="s">
-        <v>7</v>
+      <c r="C6" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D6">
+        <v>-2015</v>
       </c>
       <c r="E6">
-        <v>-2015</v>
-      </c>
-      <c r="F6">
         <v>-2016</v>
       </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -622,17 +616,17 @@
         <f t="shared" si="0"/>
         <v>https://www.flashscore.com/football/czech-republic/1-liga-2014-2015/results/</v>
       </c>
-      <c r="D7" s="2" t="s">
-        <v>7</v>
+      <c r="C7" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7">
+        <v>-2014</v>
       </c>
       <c r="E7">
-        <v>-2014</v>
-      </c>
-      <c r="F7">
         <v>-2015</v>
       </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -640,17 +634,17 @@
         <f t="shared" si="0"/>
         <v>https://www.flashscore.com/football/czech-republic/1-liga-2013-2014/results/</v>
       </c>
-      <c r="D8" s="2" t="s">
-        <v>7</v>
+      <c r="C8" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D8">
+        <v>-2013</v>
       </c>
       <c r="E8">
-        <v>-2013</v>
-      </c>
-      <c r="F8">
         <v>-2014</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -658,17 +652,17 @@
         <f t="shared" si="0"/>
         <v>https://www.flashscore.com/football/czech-republic/1-liga-2012-2013/results/</v>
       </c>
-      <c r="D9" s="2" t="s">
-        <v>7</v>
+      <c r="C9" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D9">
+        <v>-2012</v>
       </c>
       <c r="E9">
-        <v>-2012</v>
-      </c>
-      <c r="F9">
         <v>-2013</v>
       </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -676,17 +670,17 @@
         <f t="shared" si="0"/>
         <v>https://www.flashscore.com/football/czech-republic/1-liga-2011-2012/results/</v>
       </c>
-      <c r="D10" s="2" t="s">
-        <v>7</v>
+      <c r="C10" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D10">
+        <v>-2011</v>
       </c>
       <c r="E10">
-        <v>-2011</v>
-      </c>
-      <c r="F10">
         <v>-2012</v>
       </c>
     </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -694,17 +688,17 @@
         <f t="shared" si="0"/>
         <v>https://www.flashscore.com/football/czech-republic/1-liga-2010-2011/results/</v>
       </c>
-      <c r="D11" s="2" t="s">
-        <v>7</v>
+      <c r="C11" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11">
+        <v>-2010</v>
       </c>
       <c r="E11">
-        <v>-2010</v>
-      </c>
-      <c r="F11">
         <v>-2011</v>
       </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -712,17 +706,17 @@
         <f t="shared" si="0"/>
         <v>https://www.flashscore.com/football/czech-republic/division-2-2019-2020/results/</v>
       </c>
-      <c r="D12" s="2" t="s">
-        <v>8</v>
+      <c r="C12" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12">
+        <v>-2019</v>
       </c>
       <c r="E12">
-        <v>-2019</v>
-      </c>
-      <c r="F12">
         <v>-2020</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -730,17 +724,17 @@
         <f t="shared" si="0"/>
         <v>https://www.flashscore.com/football/czech-republic/division-2-2018-2019/results/</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>8</v>
+      <c r="C13" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13">
+        <v>-2018</v>
       </c>
       <c r="E13">
-        <v>-2018</v>
-      </c>
-      <c r="F13">
         <v>-2019</v>
       </c>
     </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -748,17 +742,17 @@
         <f t="shared" si="0"/>
         <v>https://www.flashscore.com/football/czech-republic/division-2-2017-2018/results/</v>
       </c>
-      <c r="D14" s="2" t="s">
-        <v>8</v>
+      <c r="C14" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14">
+        <v>-2017</v>
       </c>
       <c r="E14">
-        <v>-2017</v>
-      </c>
-      <c r="F14">
         <v>-2018</v>
       </c>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -766,17 +760,17 @@
         <f t="shared" si="0"/>
         <v>https://www.flashscore.com/football/czech-republic/division-2-2016-2017/results/</v>
       </c>
-      <c r="D15" s="2" t="s">
-        <v>8</v>
+      <c r="C15" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15">
+        <v>-2016</v>
       </c>
       <c r="E15">
-        <v>-2016</v>
-      </c>
-      <c r="F15">
         <v>-2017</v>
       </c>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -784,17 +778,17 @@
         <f t="shared" si="0"/>
         <v>https://www.flashscore.com/football/czech-republic/division-2-2015-2016/results/</v>
       </c>
-      <c r="D16" s="2" t="s">
-        <v>8</v>
+      <c r="C16" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16">
+        <v>-2015</v>
       </c>
       <c r="E16">
-        <v>-2015</v>
-      </c>
-      <c r="F16">
         <v>-2016</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -802,17 +796,17 @@
         <f t="shared" si="0"/>
         <v>https://www.flashscore.com/football/czech-republic/division-2-2014-2015/results/</v>
       </c>
-      <c r="D17" s="2" t="s">
-        <v>8</v>
+      <c r="C17" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17">
+        <v>-2014</v>
       </c>
       <c r="E17">
-        <v>-2014</v>
-      </c>
-      <c r="F17">
         <v>-2015</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -820,17 +814,17 @@
         <f t="shared" si="0"/>
         <v>https://www.flashscore.com/football/czech-republic/division-2-2013-2014/results/</v>
       </c>
-      <c r="D18" s="2" t="s">
-        <v>8</v>
+      <c r="C18" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D18">
+        <v>-2013</v>
       </c>
       <c r="E18">
-        <v>-2013</v>
-      </c>
-      <c r="F18">
         <v>-2014</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -838,17 +832,17 @@
         <f t="shared" si="0"/>
         <v>https://www.flashscore.com/football/czech-republic/division-2-2012-2013/results/</v>
       </c>
-      <c r="D19" s="2" t="s">
-        <v>8</v>
+      <c r="C19" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D19">
+        <v>-2012</v>
       </c>
       <c r="E19">
-        <v>-2012</v>
-      </c>
-      <c r="F19">
         <v>-2013</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -856,17 +850,17 @@
         <f t="shared" si="0"/>
         <v>https://www.flashscore.com/football/czech-republic/division-2-2011-2012/results/</v>
       </c>
-      <c r="D20" s="2" t="s">
-        <v>8</v>
+      <c r="C20" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20">
+        <v>-2011</v>
       </c>
       <c r="E20">
-        <v>-2011</v>
-      </c>
-      <c r="F20">
         <v>-2012</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -874,125 +868,125 @@
         <f t="shared" si="0"/>
         <v>https://www.flashscore.com/football/czech-republic/division-2-2010-2011/results/</v>
       </c>
-      <c r="D21" s="2" t="s">
-        <v>8</v>
+      <c r="C21" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="D21">
+        <v>-2010</v>
       </c>
       <c r="E21">
-        <v>-2010</v>
-      </c>
-      <c r="F21">
         <v>-2011</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>20</v>
       </c>
       <c r="B22" s="2" t="str">
-        <f>D22&amp;E22&amp;F22&amp;$G$2</f>
+        <f>C22&amp;D22&amp;E22&amp;$F$2</f>
         <v>https://www.flashscore.com/football/czech-republic/msfl-2019-2020/results/</v>
       </c>
-      <c r="D22" t="s">
-        <v>9</v>
+      <c r="C22" t="s">
+        <v>8</v>
+      </c>
+      <c r="D22">
+        <v>-2019</v>
       </c>
       <c r="E22">
-        <v>-2019</v>
-      </c>
-      <c r="F22">
         <v>-2020</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>21</v>
       </c>
       <c r="B23" s="2" t="str">
-        <f t="shared" ref="B23" si="1">D23&amp;E23&amp;F23&amp;$G$2</f>
+        <f t="shared" ref="B23" si="1">C23&amp;D23&amp;E23&amp;$F$2</f>
         <v>https://www.flashscore.com/football/czech-republic/msfl-2018-2019/results/</v>
       </c>
-      <c r="D23" t="s">
-        <v>9</v>
+      <c r="C23" t="s">
+        <v>8</v>
+      </c>
+      <c r="D23">
+        <v>-2018</v>
       </c>
       <c r="E23">
-        <v>-2018</v>
-      </c>
-      <c r="F23">
         <v>-2019</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>22</v>
       </c>
       <c r="B24" s="2" t="str">
-        <f t="shared" ref="B24" si="2">D24&amp;E24&amp;F24&amp;$G$2</f>
+        <f t="shared" ref="B24" si="2">C24&amp;D24&amp;E24&amp;$F$2</f>
         <v>https://www.flashscore.com/football/czech-republic/msfl-2017-2018/results/</v>
       </c>
-      <c r="D24" t="s">
-        <v>9</v>
+      <c r="C24" t="s">
+        <v>8</v>
+      </c>
+      <c r="D24">
+        <v>-2017</v>
       </c>
       <c r="E24">
-        <v>-2017</v>
-      </c>
-      <c r="F24">
         <v>-2018</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>23</v>
       </c>
       <c r="B25" s="2" t="str">
-        <f t="shared" ref="B25" si="3">D25&amp;E25&amp;F25&amp;$G$2</f>
+        <f t="shared" ref="B25" si="3">C25&amp;D25&amp;E25&amp;$F$2</f>
         <v>https://www.flashscore.com/football/czech-republic/msfl-2016-2017/results/</v>
       </c>
-      <c r="D25" t="s">
-        <v>9</v>
+      <c r="C25" t="s">
+        <v>8</v>
+      </c>
+      <c r="D25">
+        <v>-2016</v>
       </c>
       <c r="E25">
-        <v>-2016</v>
-      </c>
-      <c r="F25">
         <v>-2017</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>24</v>
       </c>
       <c r="B26" s="2" t="str">
-        <f t="shared" ref="B26" si="4">D26&amp;E26&amp;F26&amp;$G$2</f>
+        <f t="shared" ref="B26" si="4">C26&amp;D26&amp;E26&amp;$F$2</f>
         <v>https://www.flashscore.com/football/czech-republic/msfl-2015-2016/results/</v>
       </c>
-      <c r="D26" t="s">
-        <v>9</v>
+      <c r="C26" t="s">
+        <v>8</v>
+      </c>
+      <c r="D26">
+        <v>-2015</v>
       </c>
       <c r="E26">
-        <v>-2015</v>
-      </c>
-      <c r="F26">
         <v>-2016</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>25</v>
       </c>
       <c r="B27" s="2" t="str">
-        <f t="shared" ref="B27:B31" si="5">D27&amp;E27&amp;F27&amp;$G$2</f>
+        <f t="shared" ref="B27:B31" si="5">C27&amp;D27&amp;E27&amp;$F$2</f>
         <v>https://www.flashscore.com/football/czech-republic/msfl-2014-2015/results/</v>
       </c>
-      <c r="D27" t="s">
-        <v>9</v>
+      <c r="C27" t="s">
+        <v>8</v>
+      </c>
+      <c r="D27">
+        <v>-2014</v>
       </c>
       <c r="E27">
-        <v>-2014</v>
-      </c>
-      <c r="F27">
         <v>-2015</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -1000,17 +994,17 @@
         <f t="shared" si="5"/>
         <v>https://www.flashscore.com/football/czech-republic/msfl-2013-2014/results/</v>
       </c>
-      <c r="D28" t="s">
-        <v>9</v>
+      <c r="C28" t="s">
+        <v>8</v>
+      </c>
+      <c r="D28">
+        <v>-2013</v>
       </c>
       <c r="E28">
-        <v>-2013</v>
-      </c>
-      <c r="F28">
         <v>-2014</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -1018,17 +1012,17 @@
         <f t="shared" si="5"/>
         <v>https://www.flashscore.com/football/czech-republic/msfl-2012-2013/results/</v>
       </c>
-      <c r="D29" t="s">
-        <v>9</v>
+      <c r="C29" t="s">
+        <v>8</v>
+      </c>
+      <c r="D29">
+        <v>-2012</v>
       </c>
       <c r="E29">
-        <v>-2012</v>
-      </c>
-      <c r="F29">
         <v>-2013</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -1036,17 +1030,17 @@
         <f t="shared" si="5"/>
         <v>https://www.flashscore.com/football/czech-republic/msfl-2011-2012/results/</v>
       </c>
-      <c r="D30" t="s">
-        <v>9</v>
+      <c r="C30" t="s">
+        <v>8</v>
+      </c>
+      <c r="D30">
+        <v>-2011</v>
       </c>
       <c r="E30">
-        <v>-2011</v>
-      </c>
-      <c r="F30">
         <v>-2012</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -1054,125 +1048,125 @@
         <f t="shared" si="5"/>
         <v>https://www.flashscore.com/football/czech-republic/msfl-2010-2011/results/</v>
       </c>
-      <c r="D31" t="s">
-        <v>9</v>
+      <c r="C31" t="s">
+        <v>8</v>
+      </c>
+      <c r="D31">
+        <v>-2010</v>
       </c>
       <c r="E31">
-        <v>-2010</v>
-      </c>
-      <c r="F31">
         <v>-2011</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>30</v>
       </c>
       <c r="B32" s="2" t="str">
-        <f>D32&amp;E32&amp;F32&amp;$G$2</f>
+        <f>C32&amp;D32&amp;E32&amp;$F$2</f>
         <v>https://www.flashscore.com/football/france/ligue-1-2019-2020/results/</v>
       </c>
-      <c r="D32" s="2" t="s">
-        <v>10</v>
+      <c r="C32" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D32">
+        <v>-2019</v>
       </c>
       <c r="E32">
-        <v>-2019</v>
-      </c>
-      <c r="F32">
         <v>-2020</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>31</v>
       </c>
       <c r="B33" s="2" t="str">
-        <f t="shared" ref="B33" si="6">D33&amp;E33&amp;F33&amp;$G$2</f>
+        <f t="shared" ref="B33" si="6">C33&amp;D33&amp;E33&amp;$F$2</f>
         <v>https://www.flashscore.com/football/france/ligue-1-2018-2019/results/</v>
       </c>
-      <c r="D33" s="2" t="s">
-        <v>10</v>
+      <c r="C33" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D33">
+        <v>-2018</v>
       </c>
       <c r="E33">
-        <v>-2018</v>
-      </c>
-      <c r="F33">
         <v>-2019</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>32</v>
       </c>
       <c r="B34" s="2" t="str">
-        <f t="shared" ref="B34" si="7">D34&amp;E34&amp;F34&amp;$G$2</f>
+        <f t="shared" ref="B34" si="7">C34&amp;D34&amp;E34&amp;$F$2</f>
         <v>https://www.flashscore.com/football/france/ligue-1-2017-2018/results/</v>
       </c>
-      <c r="D34" s="2" t="s">
-        <v>10</v>
+      <c r="C34" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D34">
+        <v>-2017</v>
       </c>
       <c r="E34">
-        <v>-2017</v>
-      </c>
-      <c r="F34">
         <v>-2018</v>
       </c>
     </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>33</v>
       </c>
       <c r="B35" s="2" t="str">
-        <f t="shared" ref="B35" si="8">D35&amp;E35&amp;F35&amp;$G$2</f>
+        <f t="shared" ref="B35" si="8">C35&amp;D35&amp;E35&amp;$F$2</f>
         <v>https://www.flashscore.com/football/france/ligue-1-2016-2017/results/</v>
       </c>
-      <c r="D35" s="2" t="s">
-        <v>10</v>
+      <c r="C35" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D35">
+        <v>-2016</v>
       </c>
       <c r="E35">
-        <v>-2016</v>
-      </c>
-      <c r="F35">
         <v>-2017</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>34</v>
       </c>
       <c r="B36" s="2" t="str">
-        <f t="shared" ref="B36" si="9">D36&amp;E36&amp;F36&amp;$G$2</f>
+        <f t="shared" ref="B36" si="9">C36&amp;D36&amp;E36&amp;$F$2</f>
         <v>https://www.flashscore.com/football/france/ligue-1-2015-2016/results/</v>
       </c>
-      <c r="D36" s="2" t="s">
-        <v>10</v>
+      <c r="C36" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D36">
+        <v>-2015</v>
       </c>
       <c r="E36">
-        <v>-2015</v>
-      </c>
-      <c r="F36">
         <v>-2016</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>35</v>
       </c>
       <c r="B37" s="2" t="str">
-        <f t="shared" ref="B37:B66" si="10">D37&amp;E37&amp;F37&amp;$G$2</f>
+        <f t="shared" ref="B37:B61" si="10">C37&amp;D37&amp;E37&amp;$F$2</f>
         <v>https://www.flashscore.com/football/france/ligue-1-2014-2015/results/</v>
       </c>
-      <c r="D37" s="2" t="s">
-        <v>10</v>
+      <c r="C37" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D37">
+        <v>-2014</v>
       </c>
       <c r="E37">
-        <v>-2014</v>
-      </c>
-      <c r="F37">
         <v>-2015</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -1180,17 +1174,17 @@
         <f t="shared" si="10"/>
         <v>https://www.flashscore.com/football/france/ligue-1-2013-2014/results/</v>
       </c>
-      <c r="D38" s="2" t="s">
-        <v>10</v>
+      <c r="C38" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D38">
+        <v>-2013</v>
       </c>
       <c r="E38">
-        <v>-2013</v>
-      </c>
-      <c r="F38">
         <v>-2014</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -1198,17 +1192,17 @@
         <f t="shared" si="10"/>
         <v>https://www.flashscore.com/football/france/ligue-1-2012-2013/results/</v>
       </c>
-      <c r="D39" s="2" t="s">
-        <v>10</v>
+      <c r="C39" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D39">
+        <v>-2012</v>
       </c>
       <c r="E39">
-        <v>-2012</v>
-      </c>
-      <c r="F39">
         <v>-2013</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -1216,17 +1210,17 @@
         <f t="shared" si="10"/>
         <v>https://www.flashscore.com/football/france/ligue-1-2011-2012/results/</v>
       </c>
-      <c r="D40" s="2" t="s">
-        <v>10</v>
+      <c r="C40" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D40">
+        <v>-2011</v>
       </c>
       <c r="E40">
-        <v>-2011</v>
-      </c>
-      <c r="F40">
         <v>-2012</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -1234,17 +1228,17 @@
         <f t="shared" si="10"/>
         <v>https://www.flashscore.com/football/france/ligue-1-2010-2011/results/</v>
       </c>
-      <c r="D41" s="2" t="s">
-        <v>10</v>
+      <c r="C41" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="D41">
+        <v>-2010</v>
       </c>
       <c r="E41">
-        <v>-2010</v>
-      </c>
-      <c r="F41">
         <v>-2011</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -1252,17 +1246,17 @@
         <f t="shared" si="10"/>
         <v>https://www.flashscore.com/football/france/ligue-2-2019-2020/results/</v>
       </c>
-      <c r="D42" s="2" t="s">
-        <v>11</v>
+      <c r="C42" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D42">
+        <v>-2019</v>
       </c>
       <c r="E42">
-        <v>-2019</v>
-      </c>
-      <c r="F42">
         <v>-2020</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -1270,17 +1264,17 @@
         <f t="shared" si="10"/>
         <v>https://www.flashscore.com/football/france/ligue-2-2018-2019/results/</v>
       </c>
-      <c r="D43" s="2" t="s">
-        <v>11</v>
+      <c r="C43" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D43">
+        <v>-2018</v>
       </c>
       <c r="E43">
-        <v>-2018</v>
-      </c>
-      <c r="F43">
         <v>-2019</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -1288,17 +1282,17 @@
         <f t="shared" si="10"/>
         <v>https://www.flashscore.com/football/france/ligue-2-2017-2018/results/</v>
       </c>
-      <c r="D44" s="2" t="s">
-        <v>11</v>
+      <c r="C44" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D44">
+        <v>-2017</v>
       </c>
       <c r="E44">
-        <v>-2017</v>
-      </c>
-      <c r="F44">
         <v>-2018</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -1306,17 +1300,17 @@
         <f t="shared" si="10"/>
         <v>https://www.flashscore.com/football/france/ligue-2-2016-2017/results/</v>
       </c>
-      <c r="D45" s="2" t="s">
-        <v>11</v>
+      <c r="C45" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D45">
+        <v>-2016</v>
       </c>
       <c r="E45">
-        <v>-2016</v>
-      </c>
-      <c r="F45">
         <v>-2017</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -1324,17 +1318,17 @@
         <f t="shared" si="10"/>
         <v>https://www.flashscore.com/football/france/ligue-2-2015-2016/results/</v>
       </c>
-      <c r="D46" s="2" t="s">
-        <v>11</v>
+      <c r="C46" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D46">
+        <v>-2015</v>
       </c>
       <c r="E46">
-        <v>-2015</v>
-      </c>
-      <c r="F46">
         <v>-2016</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -1342,17 +1336,17 @@
         <f t="shared" si="10"/>
         <v>https://www.flashscore.com/football/france/ligue-2-2014-2015/results/</v>
       </c>
-      <c r="D47" s="2" t="s">
-        <v>11</v>
+      <c r="C47" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D47">
+        <v>-2014</v>
       </c>
       <c r="E47">
-        <v>-2014</v>
-      </c>
-      <c r="F47">
         <v>-2015</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A48" s="1">
         <v>46</v>
       </c>
@@ -1360,17 +1354,17 @@
         <f t="shared" si="10"/>
         <v>https://www.flashscore.com/football/france/ligue-2-2013-2014/results/</v>
       </c>
-      <c r="D48" s="2" t="s">
-        <v>11</v>
+      <c r="C48" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D48">
+        <v>-2013</v>
       </c>
       <c r="E48">
-        <v>-2013</v>
-      </c>
-      <c r="F48">
         <v>-2014</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A49" s="1">
         <v>47</v>
       </c>
@@ -1378,17 +1372,17 @@
         <f t="shared" si="10"/>
         <v>https://www.flashscore.com/football/france/ligue-2-2012-2013/results/</v>
       </c>
-      <c r="D49" s="2" t="s">
-        <v>11</v>
+      <c r="C49" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D49">
+        <v>-2012</v>
       </c>
       <c r="E49">
-        <v>-2012</v>
-      </c>
-      <c r="F49">
         <v>-2013</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A50" s="1">
         <v>48</v>
       </c>
@@ -1396,17 +1390,17 @@
         <f t="shared" si="10"/>
         <v>https://www.flashscore.com/football/france/ligue-2-2011-2012/results/</v>
       </c>
-      <c r="D50" s="2" t="s">
-        <v>11</v>
+      <c r="C50" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D50">
+        <v>-2011</v>
       </c>
       <c r="E50">
-        <v>-2011</v>
-      </c>
-      <c r="F50">
         <v>-2012</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A51" s="1">
         <v>49</v>
       </c>
@@ -1414,17 +1408,17 @@
         <f t="shared" si="10"/>
         <v>https://www.flashscore.com/football/france/ligue-2-2010-2011/results/</v>
       </c>
-      <c r="D51" s="2" t="s">
-        <v>11</v>
+      <c r="C51" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="D51">
+        <v>-2010</v>
       </c>
       <c r="E51">
-        <v>-2010</v>
-      </c>
-      <c r="F51">
         <v>-2011</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A52" s="1">
         <v>50</v>
       </c>
@@ -1432,17 +1426,17 @@
         <f t="shared" si="10"/>
         <v>https://www.flashscore.com/football/france/national-2019-2020/results/</v>
       </c>
-      <c r="D52" s="2" t="s">
-        <v>12</v>
+      <c r="C52" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D52">
+        <v>-2019</v>
       </c>
       <c r="E52">
-        <v>-2019</v>
-      </c>
-      <c r="F52">
         <v>-2020</v>
       </c>
     </row>
-    <row r="53" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A53" s="1">
         <v>51</v>
       </c>
@@ -1450,17 +1444,17 @@
         <f t="shared" si="10"/>
         <v>https://www.flashscore.com/football/france/national-2018-2019/results/</v>
       </c>
-      <c r="D53" s="2" t="s">
-        <v>12</v>
+      <c r="C53" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D53">
+        <v>-2018</v>
       </c>
       <c r="E53">
-        <v>-2018</v>
-      </c>
-      <c r="F53">
         <v>-2019</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A54" s="1">
         <v>52</v>
       </c>
@@ -1468,17 +1462,17 @@
         <f t="shared" si="10"/>
         <v>https://www.flashscore.com/football/france/national-2017-2018/results/</v>
       </c>
-      <c r="D54" s="2" t="s">
-        <v>12</v>
+      <c r="C54" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D54">
+        <v>-2017</v>
       </c>
       <c r="E54">
-        <v>-2017</v>
-      </c>
-      <c r="F54">
         <v>-2018</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A55" s="1">
         <v>53</v>
       </c>
@@ -1486,17 +1480,17 @@
         <f t="shared" si="10"/>
         <v>https://www.flashscore.com/football/france/national-2016-2017/results/</v>
       </c>
-      <c r="D55" s="2" t="s">
-        <v>12</v>
+      <c r="C55" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D55">
+        <v>-2016</v>
       </c>
       <c r="E55">
-        <v>-2016</v>
-      </c>
-      <c r="F55">
         <v>-2017</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A56" s="1">
         <v>54</v>
       </c>
@@ -1504,17 +1498,17 @@
         <f t="shared" si="10"/>
         <v>https://www.flashscore.com/football/france/national-2015-2016/results/</v>
       </c>
-      <c r="D56" s="2" t="s">
-        <v>12</v>
+      <c r="C56" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D56">
+        <v>-2015</v>
       </c>
       <c r="E56">
-        <v>-2015</v>
-      </c>
-      <c r="F56">
         <v>-2016</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A57" s="1">
         <v>55</v>
       </c>
@@ -1522,17 +1516,17 @@
         <f t="shared" si="10"/>
         <v>https://www.flashscore.com/football/france/national-2014-2015/results/</v>
       </c>
-      <c r="D57" s="2" t="s">
-        <v>12</v>
+      <c r="C57" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D57">
+        <v>-2014</v>
       </c>
       <c r="E57">
-        <v>-2014</v>
-      </c>
-      <c r="F57">
         <v>-2015</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A58" s="1">
         <v>56</v>
       </c>
@@ -1540,17 +1534,17 @@
         <f t="shared" si="10"/>
         <v>https://www.flashscore.com/football/france/national-2013-2014/results/</v>
       </c>
-      <c r="D58" s="2" t="s">
-        <v>12</v>
+      <c r="C58" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D58">
+        <v>-2013</v>
       </c>
       <c r="E58">
-        <v>-2013</v>
-      </c>
-      <c r="F58">
         <v>-2014</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A59" s="1">
         <v>57</v>
       </c>
@@ -1558,17 +1552,17 @@
         <f t="shared" si="10"/>
         <v>https://www.flashscore.com/football/france/national-2012-2013/results/</v>
       </c>
-      <c r="D59" s="2" t="s">
-        <v>12</v>
+      <c r="C59" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D59">
+        <v>-2012</v>
       </c>
       <c r="E59">
-        <v>-2012</v>
-      </c>
-      <c r="F59">
         <v>-2013</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A60" s="1">
         <v>58</v>
       </c>
@@ -1576,17 +1570,17 @@
         <f t="shared" si="10"/>
         <v>https://www.flashscore.com/football/france/national-2011-2012/results/</v>
       </c>
-      <c r="D60" s="2" t="s">
-        <v>12</v>
+      <c r="C60" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D60">
+        <v>-2011</v>
       </c>
       <c r="E60">
-        <v>-2011</v>
-      </c>
-      <c r="F60">
         <v>-2012</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A61" s="1">
         <v>59</v>
       </c>
@@ -1594,37 +1588,37 @@
         <f t="shared" si="10"/>
         <v>https://www.flashscore.com/football/france/national-2010-2011/results/</v>
       </c>
-      <c r="D61" s="2" t="s">
-        <v>12</v>
+      <c r="C61" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D61">
+        <v>-2010</v>
       </c>
       <c r="E61">
-        <v>-2010</v>
-      </c>
-      <c r="F61">
         <v>-2011</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A62" s="1">
         <v>60</v>
       </c>
       <c r="B62" s="2" t="str">
-        <f>D62&amp;E62&amp;F62&amp;$G$2</f>
-        <v>/results/</v>
-      </c>
-      <c r="D62" s="2"/>
-    </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.25">
+        <f>C62&amp;D62&amp;E62&amp;$F$2</f>
+        <v>/results/</v>
+      </c>
+      <c r="C62" s="2"/>
+    </row>
+    <row r="63" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A63" s="1">
         <v>61</v>
       </c>
       <c r="B63" s="2" t="str">
-        <f t="shared" ref="B63:B66" si="11">D63&amp;E63&amp;F63&amp;$G$2</f>
-        <v>/results/</v>
-      </c>
-      <c r="D63" s="2"/>
-    </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.25">
+        <f t="shared" ref="B63:B66" si="11">C63&amp;D63&amp;E63&amp;$F$2</f>
+        <v>/results/</v>
+      </c>
+      <c r="C63" s="2"/>
+    </row>
+    <row r="64" spans="1:5" x14ac:dyDescent="0.3">
       <c r="A64" s="1">
         <v>62</v>
       </c>
@@ -1632,9 +1626,9 @@
         <f t="shared" si="11"/>
         <v>/results/</v>
       </c>
-      <c r="D64" s="2"/>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C64" s="2"/>
+    </row>
+    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A65" s="1">
         <v>63</v>
       </c>
@@ -1642,9 +1636,9 @@
         <f t="shared" si="11"/>
         <v>/results/</v>
       </c>
-      <c r="D65" s="2"/>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C65" s="2"/>
+    </row>
+    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A66" s="1">
         <v>64</v>
       </c>
@@ -1652,19 +1646,19 @@
         <f t="shared" si="11"/>
         <v>/results/</v>
       </c>
-      <c r="D66" s="2"/>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C66" s="2"/>
+    </row>
+    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A67" s="1">
         <v>65</v>
       </c>
       <c r="B67" s="2" t="str">
-        <f t="shared" ref="B67:B130" si="12">D67&amp;E67&amp;F67&amp;$G$2</f>
-        <v>/results/</v>
-      </c>
-      <c r="D67" s="2"/>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" ref="B67:B130" si="12">C67&amp;D67&amp;E67&amp;$F$2</f>
+        <v>/results/</v>
+      </c>
+      <c r="C67" s="2"/>
+    </row>
+    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A68" s="1">
         <v>66</v>
       </c>
@@ -1672,9 +1666,9 @@
         <f t="shared" si="12"/>
         <v>/results/</v>
       </c>
-      <c r="D68" s="2"/>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C68" s="2"/>
+    </row>
+    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A69" s="1">
         <v>67</v>
       </c>
@@ -1682,9 +1676,9 @@
         <f t="shared" si="12"/>
         <v>/results/</v>
       </c>
-      <c r="D69" s="2"/>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C69" s="2"/>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A70" s="1">
         <v>68</v>
       </c>
@@ -1692,9 +1686,9 @@
         <f t="shared" si="12"/>
         <v>/results/</v>
       </c>
-      <c r="D70" s="2"/>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C70" s="2"/>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A71" s="1">
         <v>69</v>
       </c>
@@ -1702,9 +1696,9 @@
         <f t="shared" si="12"/>
         <v>/results/</v>
       </c>
-      <c r="D71" s="2"/>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C71" s="2"/>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A72" s="1">
         <v>70</v>
       </c>
@@ -1712,9 +1706,9 @@
         <f t="shared" si="12"/>
         <v>/results/</v>
       </c>
-      <c r="D72" s="2"/>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C72" s="2"/>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A73" s="1">
         <v>71</v>
       </c>
@@ -1722,9 +1716,9 @@
         <f t="shared" si="12"/>
         <v>/results/</v>
       </c>
-      <c r="D73" s="2"/>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C73" s="2"/>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A74" s="1">
         <v>72</v>
       </c>
@@ -1732,9 +1726,9 @@
         <f t="shared" si="12"/>
         <v>/results/</v>
       </c>
-      <c r="D74" s="2"/>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C74" s="2"/>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A75" s="1">
         <v>73</v>
       </c>
@@ -1742,9 +1736,9 @@
         <f t="shared" si="12"/>
         <v>/results/</v>
       </c>
-      <c r="D75" s="2"/>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C75" s="2"/>
+    </row>
+    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A76" s="1">
         <v>74</v>
       </c>
@@ -1752,9 +1746,9 @@
         <f t="shared" si="12"/>
         <v>/results/</v>
       </c>
-      <c r="D76" s="2"/>
-    </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C76" s="2"/>
+    </row>
+    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A77" s="1">
         <v>75</v>
       </c>
@@ -1762,9 +1756,9 @@
         <f t="shared" si="12"/>
         <v>/results/</v>
       </c>
-      <c r="D77" s="2"/>
-    </row>
-    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C77" s="2"/>
+    </row>
+    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A78" s="1">
         <v>76</v>
       </c>
@@ -1772,9 +1766,9 @@
         <f t="shared" si="12"/>
         <v>/results/</v>
       </c>
-      <c r="D78" s="2"/>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C78" s="2"/>
+    </row>
+    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A79" s="1">
         <v>77</v>
       </c>
@@ -1782,9 +1776,9 @@
         <f t="shared" si="12"/>
         <v>/results/</v>
       </c>
-      <c r="D79" s="2"/>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C79" s="2"/>
+    </row>
+    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A80" s="1">
         <v>78</v>
       </c>
@@ -1792,9 +1786,9 @@
         <f t="shared" si="12"/>
         <v>/results/</v>
       </c>
-      <c r="D80" s="2"/>
-    </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C80" s="2"/>
+    </row>
+    <row r="81" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A81" s="1">
         <v>79</v>
       </c>
@@ -1802,9 +1796,9 @@
         <f t="shared" si="12"/>
         <v>/results/</v>
       </c>
-      <c r="D81" s="2"/>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C81" s="2"/>
+    </row>
+    <row r="82" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A82" s="1">
         <v>80</v>
       </c>
@@ -1812,9 +1806,9 @@
         <f t="shared" si="12"/>
         <v>/results/</v>
       </c>
-      <c r="D82" s="2"/>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C82" s="2"/>
+    </row>
+    <row r="83" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A83" s="1">
         <v>81</v>
       </c>
@@ -1822,9 +1816,9 @@
         <f t="shared" si="12"/>
         <v>/results/</v>
       </c>
-      <c r="D83" s="2"/>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C83" s="2"/>
+    </row>
+    <row r="84" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A84" s="1">
         <v>82</v>
       </c>
@@ -1832,9 +1826,9 @@
         <f t="shared" si="12"/>
         <v>/results/</v>
       </c>
-      <c r="D84" s="2"/>
-    </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C84" s="2"/>
+    </row>
+    <row r="85" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A85" s="1">
         <v>83</v>
       </c>
@@ -1842,9 +1836,9 @@
         <f t="shared" si="12"/>
         <v>/results/</v>
       </c>
-      <c r="D85" s="2"/>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C85" s="2"/>
+    </row>
+    <row r="86" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A86" s="1">
         <v>84</v>
       </c>
@@ -1852,9 +1846,9 @@
         <f t="shared" si="12"/>
         <v>/results/</v>
       </c>
-      <c r="D86" s="2"/>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C86" s="2"/>
+    </row>
+    <row r="87" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A87" s="1">
         <v>85</v>
       </c>
@@ -1862,9 +1856,9 @@
         <f t="shared" si="12"/>
         <v>/results/</v>
       </c>
-      <c r="D87" s="2"/>
-    </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C87" s="2"/>
+    </row>
+    <row r="88" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A88" s="1">
         <v>86</v>
       </c>
@@ -1872,9 +1866,9 @@
         <f t="shared" si="12"/>
         <v>/results/</v>
       </c>
-      <c r="D88" s="2"/>
-    </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C88" s="2"/>
+    </row>
+    <row r="89" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A89" s="1">
         <v>87</v>
       </c>
@@ -1882,9 +1876,9 @@
         <f t="shared" si="12"/>
         <v>/results/</v>
       </c>
-      <c r="D89" s="2"/>
-    </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C89" s="2"/>
+    </row>
+    <row r="90" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A90" s="1">
         <v>88</v>
       </c>
@@ -1892,9 +1886,9 @@
         <f t="shared" si="12"/>
         <v>/results/</v>
       </c>
-      <c r="D90" s="2"/>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C90" s="2"/>
+    </row>
+    <row r="91" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A91" s="1">
         <v>89</v>
       </c>
@@ -1902,9 +1896,9 @@
         <f t="shared" si="12"/>
         <v>/results/</v>
       </c>
-      <c r="D91" s="2"/>
-    </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C91" s="2"/>
+    </row>
+    <row r="92" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A92" s="1">
         <v>90</v>
       </c>
@@ -1912,9 +1906,9 @@
         <f t="shared" si="12"/>
         <v>/results/</v>
       </c>
-      <c r="D92" s="2"/>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C92" s="2"/>
+    </row>
+    <row r="93" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A93" s="1">
         <v>91</v>
       </c>
@@ -1922,9 +1916,9 @@
         <f t="shared" si="12"/>
         <v>/results/</v>
       </c>
-      <c r="D93" s="2"/>
-    </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C93" s="2"/>
+    </row>
+    <row r="94" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A94" s="1">
         <v>92</v>
       </c>
@@ -1932,9 +1926,9 @@
         <f t="shared" si="12"/>
         <v>/results/</v>
       </c>
-      <c r="D94" s="2"/>
-    </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C94" s="2"/>
+    </row>
+    <row r="95" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A95" s="1">
         <v>93</v>
       </c>
@@ -1942,9 +1936,9 @@
         <f t="shared" si="12"/>
         <v>/results/</v>
       </c>
-      <c r="D95" s="2"/>
-    </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C95" s="2"/>
+    </row>
+    <row r="96" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A96" s="1">
         <v>94</v>
       </c>
@@ -1952,9 +1946,9 @@
         <f t="shared" si="12"/>
         <v>/results/</v>
       </c>
-      <c r="D96" s="2"/>
-    </row>
-    <row r="97" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C96" s="2"/>
+    </row>
+    <row r="97" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A97" s="1">
         <v>95</v>
       </c>
@@ -1962,9 +1956,9 @@
         <f t="shared" si="12"/>
         <v>/results/</v>
       </c>
-      <c r="D97" s="2"/>
-    </row>
-    <row r="98" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C97" s="2"/>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A98" s="1">
         <v>96</v>
       </c>
@@ -1972,9 +1966,9 @@
         <f t="shared" si="12"/>
         <v>/results/</v>
       </c>
-      <c r="D98" s="2"/>
-    </row>
-    <row r="99" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C98" s="2"/>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A99" s="1">
         <v>97</v>
       </c>
@@ -1982,9 +1976,9 @@
         <f t="shared" si="12"/>
         <v>/results/</v>
       </c>
-      <c r="D99" s="2"/>
-    </row>
-    <row r="100" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C99" s="2"/>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A100" s="1">
         <v>98</v>
       </c>
@@ -1992,9 +1986,9 @@
         <f t="shared" si="12"/>
         <v>/results/</v>
       </c>
-      <c r="D100" s="2"/>
-    </row>
-    <row r="101" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C100" s="2"/>
+    </row>
+    <row r="101" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A101" s="1">
         <v>99</v>
       </c>
@@ -2002,9 +1996,9 @@
         <f t="shared" si="12"/>
         <v>/results/</v>
       </c>
-      <c r="D101" s="2"/>
-    </row>
-    <row r="102" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C101" s="2"/>
+    </row>
+    <row r="102" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A102" s="1">
         <v>100</v>
       </c>
@@ -2012,9 +2006,9 @@
         <f t="shared" si="12"/>
         <v>/results/</v>
       </c>
-      <c r="D102" s="2"/>
-    </row>
-    <row r="103" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C102" s="2"/>
+    </row>
+    <row r="103" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A103" s="1">
         <v>101</v>
       </c>
@@ -2022,9 +2016,9 @@
         <f t="shared" si="12"/>
         <v>/results/</v>
       </c>
-      <c r="D103" s="2"/>
-    </row>
-    <row r="104" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C103" s="2"/>
+    </row>
+    <row r="104" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A104" s="1">
         <v>102</v>
       </c>
@@ -2032,9 +2026,9 @@
         <f t="shared" si="12"/>
         <v>/results/</v>
       </c>
-      <c r="D104" s="2"/>
-    </row>
-    <row r="105" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C104" s="2"/>
+    </row>
+    <row r="105" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A105" s="1">
         <v>103</v>
       </c>
@@ -2042,9 +2036,9 @@
         <f t="shared" si="12"/>
         <v>/results/</v>
       </c>
-      <c r="D105" s="2"/>
-    </row>
-    <row r="106" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C105" s="2"/>
+    </row>
+    <row r="106" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A106" s="1">
         <v>104</v>
       </c>
@@ -2052,9 +2046,9 @@
         <f t="shared" si="12"/>
         <v>/results/</v>
       </c>
-      <c r="D106" s="2"/>
-    </row>
-    <row r="107" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C106" s="2"/>
+    </row>
+    <row r="107" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A107" s="1">
         <v>105</v>
       </c>
@@ -2062,9 +2056,9 @@
         <f t="shared" si="12"/>
         <v>/results/</v>
       </c>
-      <c r="D107" s="2"/>
-    </row>
-    <row r="108" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C107" s="2"/>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A108" s="1">
         <v>106</v>
       </c>
@@ -2072,9 +2066,9 @@
         <f t="shared" si="12"/>
         <v>/results/</v>
       </c>
-      <c r="D108" s="2"/>
-    </row>
-    <row r="109" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C108" s="2"/>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A109" s="1">
         <v>107</v>
       </c>
@@ -2082,9 +2076,9 @@
         <f t="shared" si="12"/>
         <v>/results/</v>
       </c>
-      <c r="D109" s="2"/>
-    </row>
-    <row r="110" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C109" s="2"/>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A110" s="1">
         <v>108</v>
       </c>
@@ -2092,9 +2086,9 @@
         <f t="shared" si="12"/>
         <v>/results/</v>
       </c>
-      <c r="D110" s="2"/>
-    </row>
-    <row r="111" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C110" s="2"/>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A111" s="1">
         <v>109</v>
       </c>
@@ -2102,9 +2096,9 @@
         <f t="shared" si="12"/>
         <v>/results/</v>
       </c>
-      <c r="D111" s="2"/>
-    </row>
-    <row r="112" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C111" s="2"/>
+    </row>
+    <row r="112" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A112" s="1">
         <v>110</v>
       </c>
@@ -2112,9 +2106,9 @@
         <f t="shared" si="12"/>
         <v>/results/</v>
       </c>
-      <c r="D112" s="2"/>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C112" s="2"/>
+    </row>
+    <row r="113" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A113" s="1">
         <v>111</v>
       </c>
@@ -2122,9 +2116,9 @@
         <f t="shared" si="12"/>
         <v>/results/</v>
       </c>
-      <c r="D113" s="2"/>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C113" s="2"/>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A114" s="1">
         <v>112</v>
       </c>
@@ -2132,9 +2126,9 @@
         <f t="shared" si="12"/>
         <v>/results/</v>
       </c>
-      <c r="D114" s="2"/>
-    </row>
-    <row r="115" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C114" s="2"/>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A115" s="1">
         <v>113</v>
       </c>
@@ -2142,9 +2136,9 @@
         <f t="shared" si="12"/>
         <v>/results/</v>
       </c>
-      <c r="D115" s="2"/>
-    </row>
-    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C115" s="2"/>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A116" s="1">
         <v>114</v>
       </c>
@@ -2152,9 +2146,9 @@
         <f t="shared" si="12"/>
         <v>/results/</v>
       </c>
-      <c r="D116" s="2"/>
-    </row>
-    <row r="117" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C116" s="2"/>
+    </row>
+    <row r="117" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A117" s="1">
         <v>115</v>
       </c>
@@ -2162,9 +2156,9 @@
         <f t="shared" si="12"/>
         <v>/results/</v>
       </c>
-      <c r="D117" s="2"/>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C117" s="2"/>
+    </row>
+    <row r="118" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A118" s="1">
         <v>116</v>
       </c>
@@ -2172,9 +2166,9 @@
         <f t="shared" si="12"/>
         <v>/results/</v>
       </c>
-      <c r="D118" s="2"/>
-    </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C118" s="2"/>
+    </row>
+    <row r="119" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A119" s="1">
         <v>117</v>
       </c>
@@ -2182,9 +2176,9 @@
         <f t="shared" si="12"/>
         <v>/results/</v>
       </c>
-      <c r="D119" s="2"/>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C119" s="2"/>
+    </row>
+    <row r="120" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A120" s="1">
         <v>118</v>
       </c>
@@ -2192,9 +2186,9 @@
         <f t="shared" si="12"/>
         <v>/results/</v>
       </c>
-      <c r="D120" s="2"/>
-    </row>
-    <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C120" s="2"/>
+    </row>
+    <row r="121" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A121" s="1">
         <v>119</v>
       </c>
@@ -2202,9 +2196,9 @@
         <f t="shared" si="12"/>
         <v>/results/</v>
       </c>
-      <c r="D121" s="2"/>
-    </row>
-    <row r="122" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C121" s="2"/>
+    </row>
+    <row r="122" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A122" s="1">
         <v>120</v>
       </c>
@@ -2212,9 +2206,9 @@
         <f t="shared" si="12"/>
         <v>/results/</v>
       </c>
-      <c r="D122" s="2"/>
-    </row>
-    <row r="123" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C122" s="2"/>
+    </row>
+    <row r="123" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A123" s="1">
         <v>121</v>
       </c>
@@ -2222,9 +2216,9 @@
         <f t="shared" si="12"/>
         <v>/results/</v>
       </c>
-      <c r="D123" s="2"/>
-    </row>
-    <row r="124" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C123" s="2"/>
+    </row>
+    <row r="124" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A124" s="1">
         <v>122</v>
       </c>
@@ -2232,9 +2226,9 @@
         <f t="shared" si="12"/>
         <v>/results/</v>
       </c>
-      <c r="D124" s="2"/>
-    </row>
-    <row r="125" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C124" s="2"/>
+    </row>
+    <row r="125" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A125" s="1">
         <v>123</v>
       </c>
@@ -2242,9 +2236,9 @@
         <f t="shared" si="12"/>
         <v>/results/</v>
       </c>
-      <c r="D125" s="2"/>
-    </row>
-    <row r="126" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C125" s="2"/>
+    </row>
+    <row r="126" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A126" s="1">
         <v>124</v>
       </c>
@@ -2252,9 +2246,9 @@
         <f t="shared" si="12"/>
         <v>/results/</v>
       </c>
-      <c r="D126" s="2"/>
-    </row>
-    <row r="127" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C126" s="2"/>
+    </row>
+    <row r="127" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A127" s="1">
         <v>125</v>
       </c>
@@ -2262,9 +2256,9 @@
         <f t="shared" si="12"/>
         <v>/results/</v>
       </c>
-      <c r="D127" s="2"/>
-    </row>
-    <row r="128" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C127" s="2"/>
+    </row>
+    <row r="128" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A128" s="1">
         <v>126</v>
       </c>
@@ -2272,9 +2266,9 @@
         <f t="shared" si="12"/>
         <v>/results/</v>
       </c>
-      <c r="D128" s="2"/>
-    </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C128" s="2"/>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A129" s="1">
         <v>127</v>
       </c>
@@ -2282,9 +2276,9 @@
         <f t="shared" si="12"/>
         <v>/results/</v>
       </c>
-      <c r="D129" s="2"/>
-    </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C129" s="2"/>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A130" s="1">
         <v>128</v>
       </c>
@@ -2292,18 +2286,18 @@
         <f t="shared" si="12"/>
         <v>/results/</v>
       </c>
-      <c r="D130" s="2"/>
-    </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="C130" s="2"/>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A131" s="1">
         <v>129</v>
       </c>
       <c r="B131" s="2" t="str">
-        <f t="shared" ref="B131:B194" si="13">D131&amp;E131&amp;F131&amp;$G$2</f>
-        <v>/results/</v>
-      </c>
-    </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+        <f t="shared" ref="B131:B194" si="13">C131&amp;D131&amp;E131&amp;$F$2</f>
+        <v>/results/</v>
+      </c>
+    </row>
+    <row r="132" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A132" s="1">
         <v>130</v>
       </c>
@@ -2312,7 +2306,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="133" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A133" s="1">
         <v>131</v>
       </c>
@@ -2321,7 +2315,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="134" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A134" s="1">
         <v>132</v>
       </c>
@@ -2330,7 +2324,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A135" s="1">
         <v>133</v>
       </c>
@@ -2339,7 +2333,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A136" s="1">
         <v>134</v>
       </c>
@@ -2348,7 +2342,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A137" s="1">
         <v>135</v>
       </c>
@@ -2357,7 +2351,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A138" s="1">
         <v>136</v>
       </c>
@@ -2366,7 +2360,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A139" s="1">
         <v>137</v>
       </c>
@@ -2375,7 +2369,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A140" s="1">
         <v>138</v>
       </c>
@@ -2384,7 +2378,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="141" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A141" s="1">
         <v>139</v>
       </c>
@@ -2393,7 +2387,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="142" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A142" s="1">
         <v>140</v>
       </c>
@@ -2402,7 +2396,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A143" s="1">
         <v>141</v>
       </c>
@@ -2411,7 +2405,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A144" s="1">
         <v>142</v>
       </c>
@@ -2420,7 +2414,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="145" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A145" s="1">
         <v>143</v>
       </c>
@@ -2429,7 +2423,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="146" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A146" s="1">
         <v>144</v>
       </c>
@@ -2438,7 +2432,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="147" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A147" s="1">
         <v>145</v>
       </c>
@@ -2447,7 +2441,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="148" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A148" s="1">
         <v>146</v>
       </c>
@@ -2456,7 +2450,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="149" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A149" s="1">
         <v>147</v>
       </c>
@@ -2465,7 +2459,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="150" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A150" s="1">
         <v>148</v>
       </c>
@@ -2474,7 +2468,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="151" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A151" s="1">
         <v>149</v>
       </c>
@@ -2483,7 +2477,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="152" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A152" s="1">
         <v>150</v>
       </c>
@@ -2492,7 +2486,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="153" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="153" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A153" s="1">
         <v>151</v>
       </c>
@@ -2501,7 +2495,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="154" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="154" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A154" s="1">
         <v>152</v>
       </c>
@@ -2510,7 +2504,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="155" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A155" s="1">
         <v>153</v>
       </c>
@@ -2519,7 +2513,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="156" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A156" s="1">
         <v>154</v>
       </c>
@@ -2528,7 +2522,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="157" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="157" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A157" s="1">
         <v>155</v>
       </c>
@@ -2537,7 +2531,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="158" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="158" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A158" s="1">
         <v>156</v>
       </c>
@@ -2546,7 +2540,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="159" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="159" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A159" s="1">
         <v>157</v>
       </c>
@@ -2555,7 +2549,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="160" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="160" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A160" s="1">
         <v>158</v>
       </c>
@@ -2564,7 +2558,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="161" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A161" s="1">
         <v>159</v>
       </c>
@@ -2573,7 +2567,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="162" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A162" s="1">
         <v>160</v>
       </c>
@@ -2582,7 +2576,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="163" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A163" s="1">
         <v>161</v>
       </c>
@@ -2591,7 +2585,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="164" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A164" s="1">
         <v>162</v>
       </c>
@@ -2600,7 +2594,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="165" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A165" s="1">
         <v>163</v>
       </c>
@@ -2609,7 +2603,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="166" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A166" s="1">
         <v>164</v>
       </c>
@@ -2618,7 +2612,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="167" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A167" s="1">
         <v>165</v>
       </c>
@@ -2627,7 +2621,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="168" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="168" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A168" s="1">
         <v>166</v>
       </c>
@@ -2636,7 +2630,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="169" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A169" s="1">
         <v>167</v>
       </c>
@@ -2645,7 +2639,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="170" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A170" s="1">
         <v>168</v>
       </c>
@@ -2654,7 +2648,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="171" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A171" s="1">
         <v>169</v>
       </c>
@@ -2663,7 +2657,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="172" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A172" s="1">
         <v>170</v>
       </c>
@@ -2672,7 +2666,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="173" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A173" s="1">
         <v>171</v>
       </c>
@@ -2681,7 +2675,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="174" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A174" s="1">
         <v>172</v>
       </c>
@@ -2690,7 +2684,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="175" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A175" s="1">
         <v>173</v>
       </c>
@@ -2699,7 +2693,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="176" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A176" s="1">
         <v>174</v>
       </c>
@@ -2708,7 +2702,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="177" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A177" s="1">
         <v>175</v>
       </c>
@@ -2717,7 +2711,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="178" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A178" s="1">
         <v>176</v>
       </c>
@@ -2726,7 +2720,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="179" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A179" s="1">
         <v>177</v>
       </c>
@@ -2735,7 +2729,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="180" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="180" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A180" s="1">
         <v>178</v>
       </c>
@@ -2744,7 +2738,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="181" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A181" s="1">
         <v>179</v>
       </c>
@@ -2753,7 +2747,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="182" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="182" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A182" s="1">
         <v>180</v>
       </c>
@@ -2762,7 +2756,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="183" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A183" s="1">
         <v>181</v>
       </c>
@@ -2771,7 +2765,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="184" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A184" s="1">
         <v>182</v>
       </c>
@@ -2780,7 +2774,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="185" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="185" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A185" s="1">
         <v>183</v>
       </c>
@@ -2789,7 +2783,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="186" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A186" s="1">
         <v>184</v>
       </c>
@@ -2798,7 +2792,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="187" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A187" s="1">
         <v>185</v>
       </c>
@@ -2807,7 +2801,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="188" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A188" s="1">
         <v>186</v>
       </c>
@@ -2816,7 +2810,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="189" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A189" s="1">
         <v>187</v>
       </c>
@@ -2825,7 +2819,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="190" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A190" s="1">
         <v>188</v>
       </c>
@@ -2834,7 +2828,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="191" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A191" s="1">
         <v>189</v>
       </c>
@@ -2843,7 +2837,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="192" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A192" s="1">
         <v>190</v>
       </c>
@@ -2852,7 +2846,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="193" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A193" s="1">
         <v>191</v>
       </c>
@@ -2861,7 +2855,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="194" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A194" s="1">
         <v>192</v>
       </c>
@@ -2870,16 +2864,16 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="195" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A195" s="1">
         <v>193</v>
       </c>
       <c r="B195" s="2" t="str">
-        <f t="shared" ref="B195:B252" si="14">D195&amp;E195&amp;F195&amp;$G$2</f>
-        <v>/results/</v>
-      </c>
-    </row>
-    <row r="196" spans="1:2" x14ac:dyDescent="0.25">
+        <f t="shared" ref="B195:B252" si="14">C195&amp;D195&amp;E195&amp;$F$2</f>
+        <v>/results/</v>
+      </c>
+    </row>
+    <row r="196" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A196" s="1">
         <v>194</v>
       </c>
@@ -2888,7 +2882,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="197" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A197" s="1">
         <v>195</v>
       </c>
@@ -2897,7 +2891,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="198" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="198" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A198" s="1">
         <v>196</v>
       </c>
@@ -2906,7 +2900,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="199" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A199" s="1">
         <v>197</v>
       </c>
@@ -2915,7 +2909,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="200" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A200" s="1">
         <v>198</v>
       </c>
@@ -2924,7 +2918,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="201" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="201" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A201" s="1">
         <v>199</v>
       </c>
@@ -2933,7 +2927,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="202" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A202" s="1">
         <v>200</v>
       </c>
@@ -2942,7 +2936,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="203" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A203" s="1">
         <v>201</v>
       </c>
@@ -2951,7 +2945,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="204" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A204" s="1">
         <v>202</v>
       </c>
@@ -2960,7 +2954,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="205" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A205" s="1">
         <v>203</v>
       </c>
@@ -2969,7 +2963,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="206" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A206" s="1">
         <v>204</v>
       </c>
@@ -2978,7 +2972,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="207" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A207" s="1">
         <v>205</v>
       </c>
@@ -2987,7 +2981,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="208" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="208" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A208" s="1">
         <v>206</v>
       </c>
@@ -2996,7 +2990,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="209" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A209" s="1">
         <v>207</v>
       </c>
@@ -3005,7 +2999,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="210" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A210" s="1">
         <v>208</v>
       </c>
@@ -3014,7 +3008,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="211" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A211" s="1">
         <v>209</v>
       </c>
@@ -3023,7 +3017,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="212" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A212" s="1">
         <v>210</v>
       </c>
@@ -3032,7 +3026,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="213" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A213" s="1">
         <v>211</v>
       </c>
@@ -3041,7 +3035,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="214" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A214" s="1">
         <v>212</v>
       </c>
@@ -3050,7 +3044,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="215" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A215" s="1">
         <v>213</v>
       </c>
@@ -3059,7 +3053,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="216" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A216" s="1">
         <v>214</v>
       </c>
@@ -3068,7 +3062,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="217" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A217" s="1">
         <v>215</v>
       </c>
@@ -3077,7 +3071,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="218" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A218" s="1">
         <v>216</v>
       </c>
@@ -3086,7 +3080,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="219" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A219" s="1">
         <v>217</v>
       </c>
@@ -3095,7 +3089,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="220" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A220" s="1">
         <v>218</v>
       </c>
@@ -3104,7 +3098,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="221" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A221" s="1">
         <v>219</v>
       </c>
@@ -3113,7 +3107,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="222" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="222" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A222" s="1">
         <v>220</v>
       </c>
@@ -3122,7 +3116,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="223" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A223" s="1">
         <v>221</v>
       </c>
@@ -3131,7 +3125,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="224" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A224" s="1">
         <v>222</v>
       </c>
@@ -3140,7 +3134,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="225" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A225" s="1">
         <v>223</v>
       </c>
@@ -3149,7 +3143,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="226" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="226" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A226" s="1">
         <v>224</v>
       </c>
@@ -3158,7 +3152,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="227" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A227" s="1">
         <v>225</v>
       </c>
@@ -3167,7 +3161,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="228" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A228" s="1">
         <v>226</v>
       </c>
@@ -3176,7 +3170,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="229" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A229" s="1">
         <v>227</v>
       </c>
@@ -3185,7 +3179,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="230" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A230" s="1">
         <v>228</v>
       </c>
@@ -3194,7 +3188,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="231" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="231" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A231" s="1">
         <v>229</v>
       </c>
@@ -3203,7 +3197,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="232" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="232" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A232" s="1">
         <v>230</v>
       </c>
@@ -3212,7 +3206,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="233" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A233" s="1">
         <v>231</v>
       </c>
@@ -3221,7 +3215,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="234" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="234" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A234" s="1">
         <v>232</v>
       </c>
@@ -3230,7 +3224,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="235" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A235" s="1">
         <v>233</v>
       </c>
@@ -3239,7 +3233,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="236" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A236" s="1">
         <v>234</v>
       </c>
@@ -3248,7 +3242,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="237" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A237" s="1">
         <v>235</v>
       </c>
@@ -3257,7 +3251,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="238" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A238" s="1">
         <v>236</v>
       </c>
@@ -3266,7 +3260,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="239" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A239" s="1">
         <v>237</v>
       </c>
@@ -3275,7 +3269,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="240" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A240" s="1">
         <v>238</v>
       </c>
@@ -3284,7 +3278,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="241" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="241" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A241" s="1">
         <v>239</v>
       </c>
@@ -3293,7 +3287,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="242" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A242" s="1">
         <v>240</v>
       </c>
@@ -3302,7 +3296,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="243" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="243" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A243" s="1">
         <v>241</v>
       </c>
@@ -3311,7 +3305,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="244" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="244" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A244" s="1">
         <v>242</v>
       </c>
@@ -3320,7 +3314,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="245" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A245" s="1">
         <v>243</v>
       </c>
@@ -3329,7 +3323,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="246" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A246" s="1">
         <v>244</v>
       </c>
@@ -3338,7 +3332,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="247" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="247" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A247" s="1">
         <v>245</v>
       </c>
@@ -3347,7 +3341,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="248" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A248" s="1">
         <v>246</v>
       </c>
@@ -3356,7 +3350,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="249" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="249" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A249" s="1">
         <v>247</v>
       </c>
@@ -3365,7 +3359,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="250" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="250" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A250" s="1">
         <v>248</v>
       </c>
@@ -3374,7 +3368,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="251" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A251" s="1">
         <v>249</v>
       </c>
@@ -3383,7 +3377,7 @@
         <v>/results/</v>
       </c>
     </row>
-    <row r="252" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="252" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A252" s="1">
         <v>250</v>
       </c>
@@ -3400,33 +3394,33 @@
     <hyperlink ref="B12:B21" r:id="rId3" display="https://www.flashscore.com/football/albania/superliga-2019-2020/results/" xr:uid="{3493987D-1945-426E-A420-E89CD40AD655}"/>
     <hyperlink ref="B22" r:id="rId4" display="https://www.flashscore.com/football/albania/superliga-2019-2020/results/" xr:uid="{88803C16-2936-48CC-98F5-BDEEB84171FB}"/>
     <hyperlink ref="B23:B31" r:id="rId5" display="https://www.flashscore.com/football/algeria/ligue-1-" xr:uid="{37AAB01D-1421-4E5A-BEC3-33ECB0A74A4D}"/>
-    <hyperlink ref="D2" r:id="rId6" xr:uid="{787AD8FB-FAB7-4006-902C-B5F3547E7191}"/>
-    <hyperlink ref="D3:D11" r:id="rId7" display="https://www.flashscore.com/football/czech-republic/1-liga" xr:uid="{D21EBA52-2D81-4163-A2BE-8B95BB23B168}"/>
-    <hyperlink ref="D12" r:id="rId8" xr:uid="{8E476479-AF80-4D1D-BDDC-06E1AE5C2ECA}"/>
-    <hyperlink ref="D13" r:id="rId9" xr:uid="{78448471-2A30-4952-AAA6-796D4631D6D6}"/>
-    <hyperlink ref="D14" r:id="rId10" xr:uid="{545DD772-7382-4C0A-8571-3995B0FEB4C4}"/>
-    <hyperlink ref="D16" r:id="rId11" xr:uid="{1A6DC8FE-6E75-431A-8A16-4D9F3AFD0C7B}"/>
-    <hyperlink ref="D18" r:id="rId12" xr:uid="{CE80D047-38E3-45A9-A804-B9125029E8D6}"/>
-    <hyperlink ref="D20" r:id="rId13" xr:uid="{6AAC7F51-2BF9-4E49-A1D0-E079134EF736}"/>
-    <hyperlink ref="D15" r:id="rId14" xr:uid="{2FE5D9FE-5A8F-4DF0-820F-165A9B805748}"/>
-    <hyperlink ref="D17" r:id="rId15" xr:uid="{0FA4BC05-3470-43C9-A666-DE28B2D7CABC}"/>
-    <hyperlink ref="D19" r:id="rId16" xr:uid="{31052B48-BDB8-42D6-9F41-BB9ACDDE0EE0}"/>
-    <hyperlink ref="D21" r:id="rId17" xr:uid="{2A49AB25-C482-4B29-922B-9A7B04A5896C}"/>
+    <hyperlink ref="C2" r:id="rId6" xr:uid="{787AD8FB-FAB7-4006-902C-B5F3547E7191}"/>
+    <hyperlink ref="C3:C11" r:id="rId7" display="https://www.flashscore.com/football/czech-republic/1-liga" xr:uid="{D21EBA52-2D81-4163-A2BE-8B95BB23B168}"/>
+    <hyperlink ref="C12" r:id="rId8" xr:uid="{8E476479-AF80-4D1D-BDDC-06E1AE5C2ECA}"/>
+    <hyperlink ref="C13" r:id="rId9" xr:uid="{78448471-2A30-4952-AAA6-796D4631D6D6}"/>
+    <hyperlink ref="C14" r:id="rId10" xr:uid="{545DD772-7382-4C0A-8571-3995B0FEB4C4}"/>
+    <hyperlink ref="C16" r:id="rId11" xr:uid="{1A6DC8FE-6E75-431A-8A16-4D9F3AFD0C7B}"/>
+    <hyperlink ref="C18" r:id="rId12" xr:uid="{CE80D047-38E3-45A9-A804-B9125029E8D6}"/>
+    <hyperlink ref="C20" r:id="rId13" xr:uid="{6AAC7F51-2BF9-4E49-A1D0-E079134EF736}"/>
+    <hyperlink ref="C15" r:id="rId14" xr:uid="{2FE5D9FE-5A8F-4DF0-820F-165A9B805748}"/>
+    <hyperlink ref="C17" r:id="rId15" xr:uid="{0FA4BC05-3470-43C9-A666-DE28B2D7CABC}"/>
+    <hyperlink ref="C19" r:id="rId16" xr:uid="{31052B48-BDB8-42D6-9F41-BB9ACDDE0EE0}"/>
+    <hyperlink ref="C21" r:id="rId17" xr:uid="{2A49AB25-C482-4B29-922B-9A7B04A5896C}"/>
     <hyperlink ref="B32" r:id="rId18" display="https://www.flashscore.com/football/albania/superliga-2019-2020/results/" xr:uid="{87CE32E0-0590-4132-86D3-255A5CF67D8C}"/>
     <hyperlink ref="B33:B41" r:id="rId19" display="https://www.flashscore.com/football/czech-republic/division-2" xr:uid="{01BB8C53-9909-451C-9206-4FA8274C88AB}"/>
     <hyperlink ref="B62" r:id="rId20" display="https://www.flashscore.com/football/albania/superliga-2019-2020/results/" xr:uid="{1739D734-9899-449B-B559-B79E60FBE3E5}"/>
-    <hyperlink ref="D63:D71" r:id="rId21" display="https://www.flashscore.com/football/albania/superliga-" xr:uid="{21CCABB3-B02C-4EFC-BF95-EA408849CDD8}"/>
+    <hyperlink ref="C63:C71" r:id="rId21" display="https://www.flashscore.com/football/albania/superliga-" xr:uid="{21CCABB3-B02C-4EFC-BF95-EA408849CDD8}"/>
     <hyperlink ref="B63:B71" r:id="rId22" display="https://www.flashscore.com/football/czech-republic/division-2" xr:uid="{577F8FD6-A1A1-48F0-91C4-E70027DF3C52}"/>
-    <hyperlink ref="D33" r:id="rId23" xr:uid="{9DB33A26-805E-4906-BB82-5353D125A597}"/>
-    <hyperlink ref="D35" r:id="rId24" xr:uid="{3144CFDE-2608-4294-9795-AD169319E10B}"/>
-    <hyperlink ref="D37" r:id="rId25" xr:uid="{72B7E17E-1D7B-4798-B1AB-C770EE9CE812}"/>
-    <hyperlink ref="D39" r:id="rId26" xr:uid="{3A8B6F78-1355-4FD9-AE69-99A272BD63CD}"/>
-    <hyperlink ref="D41" r:id="rId27" xr:uid="{DE8FFECE-0B99-4DAE-A17A-04C05E47F834}"/>
-    <hyperlink ref="D43" r:id="rId28" xr:uid="{FF2C6AC1-D9EB-4F07-8F9D-F2BBA4960974}"/>
-    <hyperlink ref="D45" r:id="rId29" xr:uid="{09D301E8-EF97-4707-97A8-8C00D81C51AA}"/>
-    <hyperlink ref="D47" r:id="rId30" xr:uid="{F7D8AFB2-300F-453B-B43C-F79E1E8B818C}"/>
-    <hyperlink ref="D49" r:id="rId31" xr:uid="{1901699E-371E-4820-BB0B-30E6A51BD797}"/>
-    <hyperlink ref="D51" r:id="rId32" xr:uid="{4EAC4529-F332-4F77-B53F-E54837943873}"/>
+    <hyperlink ref="C33" r:id="rId23" xr:uid="{9DB33A26-805E-4906-BB82-5353D125A597}"/>
+    <hyperlink ref="C35" r:id="rId24" xr:uid="{3144CFDE-2608-4294-9795-AD169319E10B}"/>
+    <hyperlink ref="C37" r:id="rId25" xr:uid="{72B7E17E-1D7B-4798-B1AB-C770EE9CE812}"/>
+    <hyperlink ref="C39" r:id="rId26" xr:uid="{3A8B6F78-1355-4FD9-AE69-99A272BD63CD}"/>
+    <hyperlink ref="C41" r:id="rId27" xr:uid="{DE8FFECE-0B99-4DAE-A17A-04C05E47F834}"/>
+    <hyperlink ref="C43" r:id="rId28" xr:uid="{FF2C6AC1-D9EB-4F07-8F9D-F2BBA4960974}"/>
+    <hyperlink ref="C45" r:id="rId29" xr:uid="{09D301E8-EF97-4707-97A8-8C00D81C51AA}"/>
+    <hyperlink ref="C47" r:id="rId30" xr:uid="{F7D8AFB2-300F-453B-B43C-F79E1E8B818C}"/>
+    <hyperlink ref="C49" r:id="rId31" xr:uid="{1901699E-371E-4820-BB0B-30E6A51BD797}"/>
+    <hyperlink ref="C51" r:id="rId32" xr:uid="{4EAC4529-F332-4F77-B53F-E54837943873}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added loading page between two match summaries
</commit_message>
<xml_diff>
--- a/urls.xlsx
+++ b/urls.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Maciej\Desktop\python_projects\flashscore-scraper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{207B4998-54A4-4C0E-B411-49E67B1F2ECE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{13FC8268-8C1D-4377-A3ED-B8E580C0289B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -488,8 +488,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F252"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C1048576"/>
+    <sheetView tabSelected="1" topLeftCell="A17" workbookViewId="0">
+      <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1599,1792 +1599,837 @@
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A62" s="1">
-        <v>60</v>
-      </c>
-      <c r="B62" s="2" t="str">
-        <f>C62&amp;D62&amp;E62&amp;$F$2</f>
-        <v>/results/</v>
-      </c>
+      <c r="A62" s="1"/>
+      <c r="B62" s="2"/>
       <c r="C62" s="2"/>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A63" s="1">
-        <v>61</v>
-      </c>
-      <c r="B63" s="2" t="str">
-        <f t="shared" ref="B63:B66" si="11">C63&amp;D63&amp;E63&amp;$F$2</f>
-        <v>/results/</v>
-      </c>
+      <c r="A63" s="1"/>
+      <c r="B63" s="2"/>
       <c r="C63" s="2"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.3">
-      <c r="A64" s="1">
-        <v>62</v>
-      </c>
-      <c r="B64" s="2" t="str">
-        <f t="shared" si="11"/>
-        <v>/results/</v>
-      </c>
+      <c r="A64" s="1"/>
+      <c r="B64" s="2"/>
       <c r="C64" s="2"/>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A65" s="1">
-        <v>63</v>
-      </c>
-      <c r="B65" s="2" t="str">
-        <f t="shared" si="11"/>
-        <v>/results/</v>
-      </c>
+      <c r="A65" s="1"/>
+      <c r="B65" s="2"/>
       <c r="C65" s="2"/>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A66" s="1">
-        <v>64</v>
-      </c>
-      <c r="B66" s="2" t="str">
-        <f t="shared" si="11"/>
-        <v>/results/</v>
-      </c>
+      <c r="A66" s="1"/>
+      <c r="B66" s="2"/>
       <c r="C66" s="2"/>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A67" s="1">
-        <v>65</v>
-      </c>
-      <c r="B67" s="2" t="str">
-        <f t="shared" ref="B67:B130" si="12">C67&amp;D67&amp;E67&amp;$F$2</f>
-        <v>/results/</v>
-      </c>
+      <c r="A67" s="1"/>
+      <c r="B67" s="2"/>
       <c r="C67" s="2"/>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A68" s="1">
-        <v>66</v>
-      </c>
-      <c r="B68" s="2" t="str">
-        <f t="shared" si="12"/>
-        <v>/results/</v>
-      </c>
+      <c r="A68" s="1"/>
+      <c r="B68" s="2"/>
       <c r="C68" s="2"/>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A69" s="1">
-        <v>67</v>
-      </c>
-      <c r="B69" s="2" t="str">
-        <f t="shared" si="12"/>
-        <v>/results/</v>
-      </c>
+      <c r="A69" s="1"/>
+      <c r="B69" s="2"/>
       <c r="C69" s="2"/>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A70" s="1">
-        <v>68</v>
-      </c>
-      <c r="B70" s="2" t="str">
-        <f t="shared" si="12"/>
-        <v>/results/</v>
-      </c>
+      <c r="A70" s="1"/>
+      <c r="B70" s="2"/>
       <c r="C70" s="2"/>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A71" s="1">
-        <v>69</v>
-      </c>
-      <c r="B71" s="2" t="str">
-        <f t="shared" si="12"/>
-        <v>/results/</v>
-      </c>
+      <c r="A71" s="1"/>
+      <c r="B71" s="2"/>
       <c r="C71" s="2"/>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A72" s="1">
-        <v>70</v>
-      </c>
-      <c r="B72" s="2" t="str">
-        <f t="shared" si="12"/>
-        <v>/results/</v>
-      </c>
+      <c r="A72" s="1"/>
+      <c r="B72" s="2"/>
       <c r="C72" s="2"/>
     </row>
     <row r="73" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A73" s="1">
-        <v>71</v>
-      </c>
-      <c r="B73" s="2" t="str">
-        <f t="shared" si="12"/>
-        <v>/results/</v>
-      </c>
+      <c r="A73" s="1"/>
+      <c r="B73" s="2"/>
       <c r="C73" s="2"/>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A74" s="1">
-        <v>72</v>
-      </c>
-      <c r="B74" s="2" t="str">
-        <f t="shared" si="12"/>
-        <v>/results/</v>
-      </c>
+      <c r="A74" s="1"/>
+      <c r="B74" s="2"/>
       <c r="C74" s="2"/>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A75" s="1">
-        <v>73</v>
-      </c>
-      <c r="B75" s="2" t="str">
-        <f t="shared" si="12"/>
-        <v>/results/</v>
-      </c>
+      <c r="A75" s="1"/>
+      <c r="B75" s="2"/>
       <c r="C75" s="2"/>
     </row>
     <row r="76" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A76" s="1">
-        <v>74</v>
-      </c>
-      <c r="B76" s="2" t="str">
-        <f t="shared" si="12"/>
-        <v>/results/</v>
-      </c>
+      <c r="A76" s="1"/>
+      <c r="B76" s="2"/>
       <c r="C76" s="2"/>
     </row>
     <row r="77" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A77" s="1">
-        <v>75</v>
-      </c>
-      <c r="B77" s="2" t="str">
-        <f t="shared" si="12"/>
-        <v>/results/</v>
-      </c>
+      <c r="A77" s="1"/>
+      <c r="B77" s="2"/>
       <c r="C77" s="2"/>
     </row>
     <row r="78" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A78" s="1">
-        <v>76</v>
-      </c>
-      <c r="B78" s="2" t="str">
-        <f t="shared" si="12"/>
-        <v>/results/</v>
-      </c>
+      <c r="A78" s="1"/>
+      <c r="B78" s="2"/>
       <c r="C78" s="2"/>
     </row>
     <row r="79" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A79" s="1">
-        <v>77</v>
-      </c>
-      <c r="B79" s="2" t="str">
-        <f t="shared" si="12"/>
-        <v>/results/</v>
-      </c>
+      <c r="A79" s="1"/>
+      <c r="B79" s="2"/>
       <c r="C79" s="2"/>
     </row>
     <row r="80" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A80" s="1">
-        <v>78</v>
-      </c>
-      <c r="B80" s="2" t="str">
-        <f t="shared" si="12"/>
-        <v>/results/</v>
-      </c>
+      <c r="A80" s="1"/>
+      <c r="B80" s="2"/>
       <c r="C80" s="2"/>
     </row>
     <row r="81" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A81" s="1">
-        <v>79</v>
-      </c>
-      <c r="B81" s="2" t="str">
-        <f t="shared" si="12"/>
-        <v>/results/</v>
-      </c>
+      <c r="A81" s="1"/>
+      <c r="B81" s="2"/>
       <c r="C81" s="2"/>
     </row>
     <row r="82" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A82" s="1">
-        <v>80</v>
-      </c>
-      <c r="B82" s="2" t="str">
-        <f t="shared" si="12"/>
-        <v>/results/</v>
-      </c>
+      <c r="A82" s="1"/>
+      <c r="B82" s="2"/>
       <c r="C82" s="2"/>
     </row>
     <row r="83" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A83" s="1">
-        <v>81</v>
-      </c>
-      <c r="B83" s="2" t="str">
-        <f t="shared" si="12"/>
-        <v>/results/</v>
-      </c>
+      <c r="A83" s="1"/>
+      <c r="B83" s="2"/>
       <c r="C83" s="2"/>
     </row>
     <row r="84" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A84" s="1">
-        <v>82</v>
-      </c>
-      <c r="B84" s="2" t="str">
-        <f t="shared" si="12"/>
-        <v>/results/</v>
-      </c>
+      <c r="A84" s="1"/>
+      <c r="B84" s="2"/>
       <c r="C84" s="2"/>
     </row>
     <row r="85" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A85" s="1">
-        <v>83</v>
-      </c>
-      <c r="B85" s="2" t="str">
-        <f t="shared" si="12"/>
-        <v>/results/</v>
-      </c>
+      <c r="A85" s="1"/>
+      <c r="B85" s="2"/>
       <c r="C85" s="2"/>
     </row>
     <row r="86" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A86" s="1">
-        <v>84</v>
-      </c>
-      <c r="B86" s="2" t="str">
-        <f t="shared" si="12"/>
-        <v>/results/</v>
-      </c>
+      <c r="A86" s="1"/>
+      <c r="B86" s="2"/>
       <c r="C86" s="2"/>
     </row>
     <row r="87" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A87" s="1">
-        <v>85</v>
-      </c>
-      <c r="B87" s="2" t="str">
-        <f t="shared" si="12"/>
-        <v>/results/</v>
-      </c>
+      <c r="A87" s="1"/>
+      <c r="B87" s="2"/>
       <c r="C87" s="2"/>
     </row>
     <row r="88" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A88" s="1">
-        <v>86</v>
-      </c>
-      <c r="B88" s="2" t="str">
-        <f t="shared" si="12"/>
-        <v>/results/</v>
-      </c>
+      <c r="A88" s="1"/>
+      <c r="B88" s="2"/>
       <c r="C88" s="2"/>
     </row>
     <row r="89" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A89" s="1">
-        <v>87</v>
-      </c>
-      <c r="B89" s="2" t="str">
-        <f t="shared" si="12"/>
-        <v>/results/</v>
-      </c>
+      <c r="A89" s="1"/>
+      <c r="B89" s="2"/>
       <c r="C89" s="2"/>
     </row>
     <row r="90" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A90" s="1">
-        <v>88</v>
-      </c>
-      <c r="B90" s="2" t="str">
-        <f t="shared" si="12"/>
-        <v>/results/</v>
-      </c>
+      <c r="A90" s="1"/>
+      <c r="B90" s="2"/>
       <c r="C90" s="2"/>
     </row>
     <row r="91" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A91" s="1">
-        <v>89</v>
-      </c>
-      <c r="B91" s="2" t="str">
-        <f t="shared" si="12"/>
-        <v>/results/</v>
-      </c>
+      <c r="A91" s="1"/>
+      <c r="B91" s="2"/>
       <c r="C91" s="2"/>
     </row>
     <row r="92" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A92" s="1">
-        <v>90</v>
-      </c>
-      <c r="B92" s="2" t="str">
-        <f t="shared" si="12"/>
-        <v>/results/</v>
-      </c>
+      <c r="A92" s="1"/>
+      <c r="B92" s="2"/>
       <c r="C92" s="2"/>
     </row>
     <row r="93" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A93" s="1">
-        <v>91</v>
-      </c>
-      <c r="B93" s="2" t="str">
-        <f t="shared" si="12"/>
-        <v>/results/</v>
-      </c>
+      <c r="A93" s="1"/>
+      <c r="B93" s="2"/>
       <c r="C93" s="2"/>
     </row>
     <row r="94" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A94" s="1">
-        <v>92</v>
-      </c>
-      <c r="B94" s="2" t="str">
-        <f t="shared" si="12"/>
-        <v>/results/</v>
-      </c>
+      <c r="A94" s="1"/>
+      <c r="B94" s="2"/>
       <c r="C94" s="2"/>
     </row>
     <row r="95" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A95" s="1">
-        <v>93</v>
-      </c>
-      <c r="B95" s="2" t="str">
-        <f t="shared" si="12"/>
-        <v>/results/</v>
-      </c>
+      <c r="A95" s="1"/>
+      <c r="B95" s="2"/>
       <c r="C95" s="2"/>
     </row>
     <row r="96" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A96" s="1">
-        <v>94</v>
-      </c>
-      <c r="B96" s="2" t="str">
-        <f t="shared" si="12"/>
-        <v>/results/</v>
-      </c>
+      <c r="A96" s="1"/>
+      <c r="B96" s="2"/>
       <c r="C96" s="2"/>
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A97" s="1">
-        <v>95</v>
-      </c>
-      <c r="B97" s="2" t="str">
-        <f t="shared" si="12"/>
-        <v>/results/</v>
-      </c>
+      <c r="A97" s="1"/>
+      <c r="B97" s="2"/>
       <c r="C97" s="2"/>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A98" s="1">
-        <v>96</v>
-      </c>
-      <c r="B98" s="2" t="str">
-        <f t="shared" si="12"/>
-        <v>/results/</v>
-      </c>
+      <c r="A98" s="1"/>
+      <c r="B98" s="2"/>
       <c r="C98" s="2"/>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A99" s="1">
-        <v>97</v>
-      </c>
-      <c r="B99" s="2" t="str">
-        <f t="shared" si="12"/>
-        <v>/results/</v>
-      </c>
+      <c r="A99" s="1"/>
+      <c r="B99" s="2"/>
       <c r="C99" s="2"/>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A100" s="1">
-        <v>98</v>
-      </c>
-      <c r="B100" s="2" t="str">
-        <f t="shared" si="12"/>
-        <v>/results/</v>
-      </c>
+      <c r="A100" s="1"/>
+      <c r="B100" s="2"/>
       <c r="C100" s="2"/>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A101" s="1">
-        <v>99</v>
-      </c>
-      <c r="B101" s="2" t="str">
-        <f t="shared" si="12"/>
-        <v>/results/</v>
-      </c>
+      <c r="A101" s="1"/>
+      <c r="B101" s="2"/>
       <c r="C101" s="2"/>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A102" s="1">
-        <v>100</v>
-      </c>
-      <c r="B102" s="2" t="str">
-        <f t="shared" si="12"/>
-        <v>/results/</v>
-      </c>
+      <c r="A102" s="1"/>
+      <c r="B102" s="2"/>
       <c r="C102" s="2"/>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A103" s="1">
-        <v>101</v>
-      </c>
-      <c r="B103" s="2" t="str">
-        <f t="shared" si="12"/>
-        <v>/results/</v>
-      </c>
+      <c r="A103" s="1"/>
+      <c r="B103" s="2"/>
       <c r="C103" s="2"/>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A104" s="1">
-        <v>102</v>
-      </c>
-      <c r="B104" s="2" t="str">
-        <f t="shared" si="12"/>
-        <v>/results/</v>
-      </c>
+      <c r="A104" s="1"/>
+      <c r="B104" s="2"/>
       <c r="C104" s="2"/>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A105" s="1">
-        <v>103</v>
-      </c>
-      <c r="B105" s="2" t="str">
-        <f t="shared" si="12"/>
-        <v>/results/</v>
-      </c>
+      <c r="A105" s="1"/>
+      <c r="B105" s="2"/>
       <c r="C105" s="2"/>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A106" s="1">
-        <v>104</v>
-      </c>
-      <c r="B106" s="2" t="str">
-        <f t="shared" si="12"/>
-        <v>/results/</v>
-      </c>
+      <c r="A106" s="1"/>
+      <c r="B106" s="2"/>
       <c r="C106" s="2"/>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A107" s="1">
-        <v>105</v>
-      </c>
-      <c r="B107" s="2" t="str">
-        <f t="shared" si="12"/>
-        <v>/results/</v>
-      </c>
+      <c r="A107" s="1"/>
+      <c r="B107" s="2"/>
       <c r="C107" s="2"/>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A108" s="1">
-        <v>106</v>
-      </c>
-      <c r="B108" s="2" t="str">
-        <f t="shared" si="12"/>
-        <v>/results/</v>
-      </c>
+      <c r="A108" s="1"/>
+      <c r="B108" s="2"/>
       <c r="C108" s="2"/>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A109" s="1">
-        <v>107</v>
-      </c>
-      <c r="B109" s="2" t="str">
-        <f t="shared" si="12"/>
-        <v>/results/</v>
-      </c>
+      <c r="A109" s="1"/>
+      <c r="B109" s="2"/>
       <c r="C109" s="2"/>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A110" s="1">
-        <v>108</v>
-      </c>
-      <c r="B110" s="2" t="str">
-        <f t="shared" si="12"/>
-        <v>/results/</v>
-      </c>
+      <c r="A110" s="1"/>
+      <c r="B110" s="2"/>
       <c r="C110" s="2"/>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A111" s="1">
-        <v>109</v>
-      </c>
-      <c r="B111" s="2" t="str">
-        <f t="shared" si="12"/>
-        <v>/results/</v>
-      </c>
+      <c r="A111" s="1"/>
+      <c r="B111" s="2"/>
       <c r="C111" s="2"/>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A112" s="1">
-        <v>110</v>
-      </c>
-      <c r="B112" s="2" t="str">
-        <f t="shared" si="12"/>
-        <v>/results/</v>
-      </c>
+      <c r="A112" s="1"/>
+      <c r="B112" s="2"/>
       <c r="C112" s="2"/>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A113" s="1">
-        <v>111</v>
-      </c>
-      <c r="B113" s="2" t="str">
-        <f t="shared" si="12"/>
-        <v>/results/</v>
-      </c>
+      <c r="A113" s="1"/>
+      <c r="B113" s="2"/>
       <c r="C113" s="2"/>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A114" s="1">
-        <v>112</v>
-      </c>
-      <c r="B114" s="2" t="str">
-        <f t="shared" si="12"/>
-        <v>/results/</v>
-      </c>
+      <c r="A114" s="1"/>
+      <c r="B114" s="2"/>
       <c r="C114" s="2"/>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A115" s="1">
-        <v>113</v>
-      </c>
-      <c r="B115" s="2" t="str">
-        <f t="shared" si="12"/>
-        <v>/results/</v>
-      </c>
+      <c r="A115" s="1"/>
+      <c r="B115" s="2"/>
       <c r="C115" s="2"/>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A116" s="1">
-        <v>114</v>
-      </c>
-      <c r="B116" s="2" t="str">
-        <f t="shared" si="12"/>
-        <v>/results/</v>
-      </c>
+      <c r="A116" s="1"/>
+      <c r="B116" s="2"/>
       <c r="C116" s="2"/>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A117" s="1">
-        <v>115</v>
-      </c>
-      <c r="B117" s="2" t="str">
-        <f t="shared" si="12"/>
-        <v>/results/</v>
-      </c>
+      <c r="A117" s="1"/>
+      <c r="B117" s="2"/>
       <c r="C117" s="2"/>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A118" s="1">
-        <v>116</v>
-      </c>
-      <c r="B118" s="2" t="str">
-        <f t="shared" si="12"/>
-        <v>/results/</v>
-      </c>
+      <c r="A118" s="1"/>
+      <c r="B118" s="2"/>
       <c r="C118" s="2"/>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A119" s="1">
-        <v>117</v>
-      </c>
-      <c r="B119" s="2" t="str">
-        <f t="shared" si="12"/>
-        <v>/results/</v>
-      </c>
+      <c r="A119" s="1"/>
+      <c r="B119" s="2"/>
       <c r="C119" s="2"/>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A120" s="1">
-        <v>118</v>
-      </c>
-      <c r="B120" s="2" t="str">
-        <f t="shared" si="12"/>
-        <v>/results/</v>
-      </c>
+      <c r="A120" s="1"/>
+      <c r="B120" s="2"/>
       <c r="C120" s="2"/>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A121" s="1">
-        <v>119</v>
-      </c>
-      <c r="B121" s="2" t="str">
-        <f t="shared" si="12"/>
-        <v>/results/</v>
-      </c>
+      <c r="A121" s="1"/>
+      <c r="B121" s="2"/>
       <c r="C121" s="2"/>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A122" s="1">
-        <v>120</v>
-      </c>
-      <c r="B122" s="2" t="str">
-        <f t="shared" si="12"/>
-        <v>/results/</v>
-      </c>
+      <c r="A122" s="1"/>
+      <c r="B122" s="2"/>
       <c r="C122" s="2"/>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A123" s="1">
-        <v>121</v>
-      </c>
-      <c r="B123" s="2" t="str">
-        <f t="shared" si="12"/>
-        <v>/results/</v>
-      </c>
+      <c r="A123" s="1"/>
+      <c r="B123" s="2"/>
       <c r="C123" s="2"/>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A124" s="1">
-        <v>122</v>
-      </c>
-      <c r="B124" s="2" t="str">
-        <f t="shared" si="12"/>
-        <v>/results/</v>
-      </c>
+      <c r="A124" s="1"/>
+      <c r="B124" s="2"/>
       <c r="C124" s="2"/>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A125" s="1">
-        <v>123</v>
-      </c>
-      <c r="B125" s="2" t="str">
-        <f t="shared" si="12"/>
-        <v>/results/</v>
-      </c>
+      <c r="A125" s="1"/>
+      <c r="B125" s="2"/>
       <c r="C125" s="2"/>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A126" s="1">
-        <v>124</v>
-      </c>
-      <c r="B126" s="2" t="str">
-        <f t="shared" si="12"/>
-        <v>/results/</v>
-      </c>
+      <c r="A126" s="1"/>
+      <c r="B126" s="2"/>
       <c r="C126" s="2"/>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A127" s="1">
-        <v>125</v>
-      </c>
-      <c r="B127" s="2" t="str">
-        <f t="shared" si="12"/>
-        <v>/results/</v>
-      </c>
+      <c r="A127" s="1"/>
+      <c r="B127" s="2"/>
       <c r="C127" s="2"/>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A128" s="1">
-        <v>126</v>
-      </c>
-      <c r="B128" s="2" t="str">
-        <f t="shared" si="12"/>
-        <v>/results/</v>
-      </c>
+      <c r="A128" s="1"/>
+      <c r="B128" s="2"/>
       <c r="C128" s="2"/>
     </row>
     <row r="129" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A129" s="1">
-        <v>127</v>
-      </c>
-      <c r="B129" s="2" t="str">
-        <f t="shared" si="12"/>
-        <v>/results/</v>
-      </c>
+      <c r="A129" s="1"/>
+      <c r="B129" s="2"/>
       <c r="C129" s="2"/>
     </row>
     <row r="130" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A130" s="1">
-        <v>128</v>
-      </c>
-      <c r="B130" s="2" t="str">
-        <f t="shared" si="12"/>
-        <v>/results/</v>
-      </c>
+      <c r="A130" s="1"/>
+      <c r="B130" s="2"/>
       <c r="C130" s="2"/>
     </row>
     <row r="131" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A131" s="1">
-        <v>129</v>
-      </c>
-      <c r="B131" s="2" t="str">
-        <f t="shared" ref="B131:B194" si="13">C131&amp;D131&amp;E131&amp;$F$2</f>
-        <v>/results/</v>
-      </c>
+      <c r="A131" s="1"/>
+      <c r="B131" s="2"/>
     </row>
     <row r="132" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A132" s="1">
-        <v>130</v>
-      </c>
-      <c r="B132" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>/results/</v>
-      </c>
+      <c r="A132" s="1"/>
+      <c r="B132" s="2"/>
     </row>
     <row r="133" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A133" s="1">
-        <v>131</v>
-      </c>
-      <c r="B133" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>/results/</v>
-      </c>
+      <c r="A133" s="1"/>
+      <c r="B133" s="2"/>
     </row>
     <row r="134" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A134" s="1">
-        <v>132</v>
-      </c>
-      <c r="B134" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>/results/</v>
-      </c>
+      <c r="A134" s="1"/>
+      <c r="B134" s="2"/>
     </row>
     <row r="135" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A135" s="1">
-        <v>133</v>
-      </c>
-      <c r="B135" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>/results/</v>
-      </c>
+      <c r="A135" s="1"/>
+      <c r="B135" s="2"/>
     </row>
     <row r="136" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A136" s="1">
-        <v>134</v>
-      </c>
-      <c r="B136" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>/results/</v>
-      </c>
+      <c r="A136" s="1"/>
+      <c r="B136" s="2"/>
     </row>
     <row r="137" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A137" s="1">
-        <v>135</v>
-      </c>
-      <c r="B137" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>/results/</v>
-      </c>
+      <c r="A137" s="1"/>
+      <c r="B137" s="2"/>
     </row>
     <row r="138" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A138" s="1">
-        <v>136</v>
-      </c>
-      <c r="B138" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>/results/</v>
-      </c>
+      <c r="A138" s="1"/>
+      <c r="B138" s="2"/>
     </row>
     <row r="139" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A139" s="1">
-        <v>137</v>
-      </c>
-      <c r="B139" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>/results/</v>
-      </c>
+      <c r="A139" s="1"/>
+      <c r="B139" s="2"/>
     </row>
     <row r="140" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A140" s="1">
-        <v>138</v>
-      </c>
-      <c r="B140" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>/results/</v>
-      </c>
+      <c r="A140" s="1"/>
+      <c r="B140" s="2"/>
     </row>
     <row r="141" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A141" s="1">
-        <v>139</v>
-      </c>
-      <c r="B141" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>/results/</v>
-      </c>
+      <c r="A141" s="1"/>
+      <c r="B141" s="2"/>
     </row>
     <row r="142" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A142" s="1">
-        <v>140</v>
-      </c>
-      <c r="B142" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>/results/</v>
-      </c>
+      <c r="A142" s="1"/>
+      <c r="B142" s="2"/>
     </row>
     <row r="143" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A143" s="1">
-        <v>141</v>
-      </c>
-      <c r="B143" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>/results/</v>
-      </c>
+      <c r="A143" s="1"/>
+      <c r="B143" s="2"/>
     </row>
     <row r="144" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A144" s="1">
-        <v>142</v>
-      </c>
-      <c r="B144" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>/results/</v>
-      </c>
+      <c r="A144" s="1"/>
+      <c r="B144" s="2"/>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A145" s="1">
-        <v>143</v>
-      </c>
-      <c r="B145" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>/results/</v>
-      </c>
+      <c r="A145" s="1"/>
+      <c r="B145" s="2"/>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A146" s="1">
-        <v>144</v>
-      </c>
-      <c r="B146" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>/results/</v>
-      </c>
+      <c r="A146" s="1"/>
+      <c r="B146" s="2"/>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A147" s="1">
-        <v>145</v>
-      </c>
-      <c r="B147" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>/results/</v>
-      </c>
+      <c r="A147" s="1"/>
+      <c r="B147" s="2"/>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A148" s="1">
-        <v>146</v>
-      </c>
-      <c r="B148" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>/results/</v>
-      </c>
+      <c r="A148" s="1"/>
+      <c r="B148" s="2"/>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A149" s="1">
-        <v>147</v>
-      </c>
-      <c r="B149" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>/results/</v>
-      </c>
+      <c r="A149" s="1"/>
+      <c r="B149" s="2"/>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A150" s="1">
-        <v>148</v>
-      </c>
-      <c r="B150" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>/results/</v>
-      </c>
+      <c r="A150" s="1"/>
+      <c r="B150" s="2"/>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A151" s="1">
-        <v>149</v>
-      </c>
-      <c r="B151" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>/results/</v>
-      </c>
+      <c r="A151" s="1"/>
+      <c r="B151" s="2"/>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A152" s="1">
-        <v>150</v>
-      </c>
-      <c r="B152" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>/results/</v>
-      </c>
+      <c r="A152" s="1"/>
+      <c r="B152" s="2"/>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A153" s="1">
-        <v>151</v>
-      </c>
-      <c r="B153" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>/results/</v>
-      </c>
+      <c r="A153" s="1"/>
+      <c r="B153" s="2"/>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A154" s="1">
-        <v>152</v>
-      </c>
-      <c r="B154" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>/results/</v>
-      </c>
+      <c r="A154" s="1"/>
+      <c r="B154" s="2"/>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A155" s="1">
-        <v>153</v>
-      </c>
-      <c r="B155" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>/results/</v>
-      </c>
+      <c r="A155" s="1"/>
+      <c r="B155" s="2"/>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A156" s="1">
-        <v>154</v>
-      </c>
-      <c r="B156" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>/results/</v>
-      </c>
+      <c r="A156" s="1"/>
+      <c r="B156" s="2"/>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A157" s="1">
-        <v>155</v>
-      </c>
-      <c r="B157" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>/results/</v>
-      </c>
+      <c r="A157" s="1"/>
+      <c r="B157" s="2"/>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A158" s="1">
-        <v>156</v>
-      </c>
-      <c r="B158" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>/results/</v>
-      </c>
+      <c r="A158" s="1"/>
+      <c r="B158" s="2"/>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A159" s="1">
-        <v>157</v>
-      </c>
-      <c r="B159" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>/results/</v>
-      </c>
+      <c r="A159" s="1"/>
+      <c r="B159" s="2"/>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A160" s="1">
-        <v>158</v>
-      </c>
-      <c r="B160" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>/results/</v>
-      </c>
+      <c r="A160" s="1"/>
+      <c r="B160" s="2"/>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A161" s="1">
-        <v>159</v>
-      </c>
-      <c r="B161" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>/results/</v>
-      </c>
+      <c r="A161" s="1"/>
+      <c r="B161" s="2"/>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A162" s="1">
-        <v>160</v>
-      </c>
-      <c r="B162" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>/results/</v>
-      </c>
+      <c r="A162" s="1"/>
+      <c r="B162" s="2"/>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A163" s="1">
-        <v>161</v>
-      </c>
-      <c r="B163" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>/results/</v>
-      </c>
+      <c r="A163" s="1"/>
+      <c r="B163" s="2"/>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A164" s="1">
-        <v>162</v>
-      </c>
-      <c r="B164" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>/results/</v>
-      </c>
+      <c r="A164" s="1"/>
+      <c r="B164" s="2"/>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A165" s="1">
-        <v>163</v>
-      </c>
-      <c r="B165" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>/results/</v>
-      </c>
+      <c r="A165" s="1"/>
+      <c r="B165" s="2"/>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A166" s="1">
-        <v>164</v>
-      </c>
-      <c r="B166" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>/results/</v>
-      </c>
+      <c r="A166" s="1"/>
+      <c r="B166" s="2"/>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A167" s="1">
-        <v>165</v>
-      </c>
-      <c r="B167" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>/results/</v>
-      </c>
+      <c r="A167" s="1"/>
+      <c r="B167" s="2"/>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A168" s="1">
-        <v>166</v>
-      </c>
-      <c r="B168" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>/results/</v>
-      </c>
+      <c r="A168" s="1"/>
+      <c r="B168" s="2"/>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A169" s="1">
-        <v>167</v>
-      </c>
-      <c r="B169" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>/results/</v>
-      </c>
+      <c r="A169" s="1"/>
+      <c r="B169" s="2"/>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A170" s="1">
-        <v>168</v>
-      </c>
-      <c r="B170" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>/results/</v>
-      </c>
+      <c r="A170" s="1"/>
+      <c r="B170" s="2"/>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A171" s="1">
-        <v>169</v>
-      </c>
-      <c r="B171" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>/results/</v>
-      </c>
+      <c r="A171" s="1"/>
+      <c r="B171" s="2"/>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A172" s="1">
-        <v>170</v>
-      </c>
-      <c r="B172" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>/results/</v>
-      </c>
+      <c r="A172" s="1"/>
+      <c r="B172" s="2"/>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A173" s="1">
-        <v>171</v>
-      </c>
-      <c r="B173" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>/results/</v>
-      </c>
+      <c r="A173" s="1"/>
+      <c r="B173" s="2"/>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A174" s="1">
-        <v>172</v>
-      </c>
-      <c r="B174" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>/results/</v>
-      </c>
+      <c r="A174" s="1"/>
+      <c r="B174" s="2"/>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A175" s="1">
-        <v>173</v>
-      </c>
-      <c r="B175" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>/results/</v>
-      </c>
+      <c r="A175" s="1"/>
+      <c r="B175" s="2"/>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A176" s="1">
-        <v>174</v>
-      </c>
-      <c r="B176" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>/results/</v>
-      </c>
+      <c r="A176" s="1"/>
+      <c r="B176" s="2"/>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A177" s="1">
-        <v>175</v>
-      </c>
-      <c r="B177" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>/results/</v>
-      </c>
+      <c r="A177" s="1"/>
+      <c r="B177" s="2"/>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A178" s="1">
-        <v>176</v>
-      </c>
-      <c r="B178" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>/results/</v>
-      </c>
+      <c r="A178" s="1"/>
+      <c r="B178" s="2"/>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A179" s="1">
-        <v>177</v>
-      </c>
-      <c r="B179" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>/results/</v>
-      </c>
+      <c r="A179" s="1"/>
+      <c r="B179" s="2"/>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A180" s="1">
-        <v>178</v>
-      </c>
-      <c r="B180" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>/results/</v>
-      </c>
+      <c r="A180" s="1"/>
+      <c r="B180" s="2"/>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A181" s="1">
-        <v>179</v>
-      </c>
-      <c r="B181" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>/results/</v>
-      </c>
+      <c r="A181" s="1"/>
+      <c r="B181" s="2"/>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A182" s="1">
-        <v>180</v>
-      </c>
-      <c r="B182" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>/results/</v>
-      </c>
+      <c r="A182" s="1"/>
+      <c r="B182" s="2"/>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A183" s="1">
-        <v>181</v>
-      </c>
-      <c r="B183" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>/results/</v>
-      </c>
+      <c r="A183" s="1"/>
+      <c r="B183" s="2"/>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A184" s="1">
-        <v>182</v>
-      </c>
-      <c r="B184" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>/results/</v>
-      </c>
+      <c r="A184" s="1"/>
+      <c r="B184" s="2"/>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A185" s="1">
-        <v>183</v>
-      </c>
-      <c r="B185" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>/results/</v>
-      </c>
+      <c r="A185" s="1"/>
+      <c r="B185" s="2"/>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A186" s="1">
-        <v>184</v>
-      </c>
-      <c r="B186" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>/results/</v>
-      </c>
+      <c r="A186" s="1"/>
+      <c r="B186" s="2"/>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A187" s="1">
-        <v>185</v>
-      </c>
-      <c r="B187" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>/results/</v>
-      </c>
+      <c r="A187" s="1"/>
+      <c r="B187" s="2"/>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A188" s="1">
-        <v>186</v>
-      </c>
-      <c r="B188" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>/results/</v>
-      </c>
+      <c r="A188" s="1"/>
+      <c r="B188" s="2"/>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A189" s="1">
-        <v>187</v>
-      </c>
-      <c r="B189" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>/results/</v>
-      </c>
+      <c r="A189" s="1"/>
+      <c r="B189" s="2"/>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A190" s="1">
-        <v>188</v>
-      </c>
-      <c r="B190" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>/results/</v>
-      </c>
+      <c r="A190" s="1"/>
+      <c r="B190" s="2"/>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A191" s="1">
-        <v>189</v>
-      </c>
-      <c r="B191" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>/results/</v>
-      </c>
+      <c r="A191" s="1"/>
+      <c r="B191" s="2"/>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A192" s="1">
-        <v>190</v>
-      </c>
-      <c r="B192" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>/results/</v>
-      </c>
+      <c r="A192" s="1"/>
+      <c r="B192" s="2"/>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A193" s="1">
-        <v>191</v>
-      </c>
-      <c r="B193" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>/results/</v>
-      </c>
+      <c r="A193" s="1"/>
+      <c r="B193" s="2"/>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A194" s="1">
-        <v>192</v>
-      </c>
-      <c r="B194" s="2" t="str">
-        <f t="shared" si="13"/>
-        <v>/results/</v>
-      </c>
+      <c r="A194" s="1"/>
+      <c r="B194" s="2"/>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A195" s="1">
-        <v>193</v>
-      </c>
-      <c r="B195" s="2" t="str">
-        <f t="shared" ref="B195:B252" si="14">C195&amp;D195&amp;E195&amp;$F$2</f>
-        <v>/results/</v>
-      </c>
+      <c r="A195" s="1"/>
+      <c r="B195" s="2"/>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A196" s="1">
-        <v>194</v>
-      </c>
-      <c r="B196" s="2" t="str">
-        <f t="shared" si="14"/>
-        <v>/results/</v>
-      </c>
+      <c r="A196" s="1"/>
+      <c r="B196" s="2"/>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A197" s="1">
-        <v>195</v>
-      </c>
-      <c r="B197" s="2" t="str">
-        <f t="shared" si="14"/>
-        <v>/results/</v>
-      </c>
+      <c r="A197" s="1"/>
+      <c r="B197" s="2"/>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A198" s="1">
-        <v>196</v>
-      </c>
-      <c r="B198" s="2" t="str">
-        <f t="shared" si="14"/>
-        <v>/results/</v>
-      </c>
+      <c r="A198" s="1"/>
+      <c r="B198" s="2"/>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A199" s="1">
-        <v>197</v>
-      </c>
-      <c r="B199" s="2" t="str">
-        <f t="shared" si="14"/>
-        <v>/results/</v>
-      </c>
+      <c r="A199" s="1"/>
+      <c r="B199" s="2"/>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A200" s="1">
-        <v>198</v>
-      </c>
-      <c r="B200" s="2" t="str">
-        <f t="shared" si="14"/>
-        <v>/results/</v>
-      </c>
+      <c r="A200" s="1"/>
+      <c r="B200" s="2"/>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A201" s="1">
-        <v>199</v>
-      </c>
-      <c r="B201" s="2" t="str">
-        <f t="shared" si="14"/>
-        <v>/results/</v>
-      </c>
+      <c r="A201" s="1"/>
+      <c r="B201" s="2"/>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A202" s="1">
-        <v>200</v>
-      </c>
-      <c r="B202" s="2" t="str">
-        <f t="shared" si="14"/>
-        <v>/results/</v>
-      </c>
+      <c r="A202" s="1"/>
+      <c r="B202" s="2"/>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A203" s="1">
-        <v>201</v>
-      </c>
-      <c r="B203" s="2" t="str">
-        <f t="shared" si="14"/>
-        <v>/results/</v>
-      </c>
+      <c r="A203" s="1"/>
+      <c r="B203" s="2"/>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A204" s="1">
-        <v>202</v>
-      </c>
-      <c r="B204" s="2" t="str">
-        <f t="shared" si="14"/>
-        <v>/results/</v>
-      </c>
+      <c r="A204" s="1"/>
+      <c r="B204" s="2"/>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A205" s="1">
-        <v>203</v>
-      </c>
-      <c r="B205" s="2" t="str">
-        <f t="shared" si="14"/>
-        <v>/results/</v>
-      </c>
+      <c r="A205" s="1"/>
+      <c r="B205" s="2"/>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A206" s="1">
-        <v>204</v>
-      </c>
-      <c r="B206" s="2" t="str">
-        <f t="shared" si="14"/>
-        <v>/results/</v>
-      </c>
+      <c r="A206" s="1"/>
+      <c r="B206" s="2"/>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A207" s="1">
-        <v>205</v>
-      </c>
-      <c r="B207" s="2" t="str">
-        <f t="shared" si="14"/>
-        <v>/results/</v>
-      </c>
+      <c r="A207" s="1"/>
+      <c r="B207" s="2"/>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A208" s="1">
-        <v>206</v>
-      </c>
-      <c r="B208" s="2" t="str">
-        <f t="shared" si="14"/>
-        <v>/results/</v>
-      </c>
+      <c r="A208" s="1"/>
+      <c r="B208" s="2"/>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A209" s="1">
-        <v>207</v>
-      </c>
-      <c r="B209" s="2" t="str">
-        <f t="shared" si="14"/>
-        <v>/results/</v>
-      </c>
+      <c r="A209" s="1"/>
+      <c r="B209" s="2"/>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A210" s="1">
-        <v>208</v>
-      </c>
-      <c r="B210" s="2" t="str">
-        <f t="shared" si="14"/>
-        <v>/results/</v>
-      </c>
+      <c r="A210" s="1"/>
+      <c r="B210" s="2"/>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A211" s="1">
-        <v>209</v>
-      </c>
-      <c r="B211" s="2" t="str">
-        <f t="shared" si="14"/>
-        <v>/results/</v>
-      </c>
+      <c r="A211" s="1"/>
+      <c r="B211" s="2"/>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A212" s="1">
-        <v>210</v>
-      </c>
-      <c r="B212" s="2" t="str">
-        <f t="shared" si="14"/>
-        <v>/results/</v>
-      </c>
+      <c r="A212" s="1"/>
+      <c r="B212" s="2"/>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A213" s="1">
-        <v>211</v>
-      </c>
-      <c r="B213" s="2" t="str">
-        <f t="shared" si="14"/>
-        <v>/results/</v>
-      </c>
+      <c r="A213" s="1"/>
+      <c r="B213" s="2"/>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A214" s="1">
-        <v>212</v>
-      </c>
-      <c r="B214" s="2" t="str">
-        <f t="shared" si="14"/>
-        <v>/results/</v>
-      </c>
+      <c r="A214" s="1"/>
+      <c r="B214" s="2"/>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A215" s="1">
-        <v>213</v>
-      </c>
-      <c r="B215" s="2" t="str">
-        <f t="shared" si="14"/>
-        <v>/results/</v>
-      </c>
+      <c r="A215" s="1"/>
+      <c r="B215" s="2"/>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A216" s="1">
-        <v>214</v>
-      </c>
-      <c r="B216" s="2" t="str">
-        <f t="shared" si="14"/>
-        <v>/results/</v>
-      </c>
+      <c r="A216" s="1"/>
+      <c r="B216" s="2"/>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A217" s="1">
-        <v>215</v>
-      </c>
-      <c r="B217" s="2" t="str">
-        <f t="shared" si="14"/>
-        <v>/results/</v>
-      </c>
+      <c r="A217" s="1"/>
+      <c r="B217" s="2"/>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A218" s="1">
-        <v>216</v>
-      </c>
-      <c r="B218" s="2" t="str">
-        <f t="shared" si="14"/>
-        <v>/results/</v>
-      </c>
+      <c r="A218" s="1"/>
+      <c r="B218" s="2"/>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A219" s="1">
-        <v>217</v>
-      </c>
-      <c r="B219" s="2" t="str">
-        <f t="shared" si="14"/>
-        <v>/results/</v>
-      </c>
+      <c r="A219" s="1"/>
+      <c r="B219" s="2"/>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A220" s="1">
-        <v>218</v>
-      </c>
-      <c r="B220" s="2" t="str">
-        <f t="shared" si="14"/>
-        <v>/results/</v>
-      </c>
+      <c r="A220" s="1"/>
+      <c r="B220" s="2"/>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A221" s="1">
-        <v>219</v>
-      </c>
-      <c r="B221" s="2" t="str">
-        <f t="shared" si="14"/>
-        <v>/results/</v>
-      </c>
+      <c r="A221" s="1"/>
+      <c r="B221" s="2"/>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A222" s="1">
-        <v>220</v>
-      </c>
-      <c r="B222" s="2" t="str">
-        <f t="shared" si="14"/>
-        <v>/results/</v>
-      </c>
+      <c r="A222" s="1"/>
+      <c r="B222" s="2"/>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A223" s="1">
-        <v>221</v>
-      </c>
-      <c r="B223" s="2" t="str">
-        <f t="shared" si="14"/>
-        <v>/results/</v>
-      </c>
+      <c r="A223" s="1"/>
+      <c r="B223" s="2"/>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A224" s="1">
-        <v>222</v>
-      </c>
-      <c r="B224" s="2" t="str">
-        <f t="shared" si="14"/>
-        <v>/results/</v>
-      </c>
+      <c r="A224" s="1"/>
+      <c r="B224" s="2"/>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A225" s="1">
-        <v>223</v>
-      </c>
-      <c r="B225" s="2" t="str">
-        <f t="shared" si="14"/>
-        <v>/results/</v>
-      </c>
+      <c r="A225" s="1"/>
+      <c r="B225" s="2"/>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A226" s="1">
-        <v>224</v>
-      </c>
-      <c r="B226" s="2" t="str">
-        <f t="shared" si="14"/>
-        <v>/results/</v>
-      </c>
+      <c r="A226" s="1"/>
+      <c r="B226" s="2"/>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A227" s="1">
-        <v>225</v>
-      </c>
-      <c r="B227" s="2" t="str">
-        <f t="shared" si="14"/>
-        <v>/results/</v>
-      </c>
+      <c r="A227" s="1"/>
+      <c r="B227" s="2"/>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A228" s="1">
-        <v>226</v>
-      </c>
-      <c r="B228" s="2" t="str">
-        <f t="shared" si="14"/>
-        <v>/results/</v>
-      </c>
+      <c r="A228" s="1"/>
+      <c r="B228" s="2"/>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A229" s="1">
-        <v>227</v>
-      </c>
-      <c r="B229" s="2" t="str">
-        <f t="shared" si="14"/>
-        <v>/results/</v>
-      </c>
+      <c r="A229" s="1"/>
+      <c r="B229" s="2"/>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A230" s="1">
-        <v>228</v>
-      </c>
-      <c r="B230" s="2" t="str">
-        <f t="shared" si="14"/>
-        <v>/results/</v>
-      </c>
+      <c r="A230" s="1"/>
+      <c r="B230" s="2"/>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A231" s="1">
-        <v>229</v>
-      </c>
-      <c r="B231" s="2" t="str">
-        <f t="shared" si="14"/>
-        <v>/results/</v>
-      </c>
+      <c r="A231" s="1"/>
+      <c r="B231" s="2"/>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A232" s="1">
-        <v>230</v>
-      </c>
-      <c r="B232" s="2" t="str">
-        <f t="shared" si="14"/>
-        <v>/results/</v>
-      </c>
+      <c r="A232" s="1"/>
+      <c r="B232" s="2"/>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A233" s="1">
-        <v>231</v>
-      </c>
-      <c r="B233" s="2" t="str">
-        <f t="shared" si="14"/>
-        <v>/results/</v>
-      </c>
+      <c r="A233" s="1"/>
+      <c r="B233" s="2"/>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A234" s="1">
-        <v>232</v>
-      </c>
-      <c r="B234" s="2" t="str">
-        <f t="shared" si="14"/>
-        <v>/results/</v>
-      </c>
+      <c r="A234" s="1"/>
+      <c r="B234" s="2"/>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A235" s="1">
-        <v>233</v>
-      </c>
-      <c r="B235" s="2" t="str">
-        <f t="shared" si="14"/>
-        <v>/results/</v>
-      </c>
+      <c r="A235" s="1"/>
+      <c r="B235" s="2"/>
     </row>
     <row r="236" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A236" s="1">
-        <v>234</v>
-      </c>
-      <c r="B236" s="2" t="str">
-        <f t="shared" si="14"/>
-        <v>/results/</v>
-      </c>
+      <c r="A236" s="1"/>
+      <c r="B236" s="2"/>
     </row>
     <row r="237" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A237" s="1">
-        <v>235</v>
-      </c>
-      <c r="B237" s="2" t="str">
-        <f t="shared" si="14"/>
-        <v>/results/</v>
-      </c>
+      <c r="A237" s="1"/>
+      <c r="B237" s="2"/>
     </row>
     <row r="238" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A238" s="1">
-        <v>236</v>
-      </c>
-      <c r="B238" s="2" t="str">
-        <f t="shared" si="14"/>
-        <v>/results/</v>
-      </c>
+      <c r="A238" s="1"/>
+      <c r="B238" s="2"/>
     </row>
     <row r="239" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A239" s="1">
-        <v>237</v>
-      </c>
-      <c r="B239" s="2" t="str">
-        <f t="shared" si="14"/>
-        <v>/results/</v>
-      </c>
+      <c r="A239" s="1"/>
+      <c r="B239" s="2"/>
     </row>
     <row r="240" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A240" s="1">
-        <v>238</v>
-      </c>
-      <c r="B240" s="2" t="str">
-        <f t="shared" si="14"/>
-        <v>/results/</v>
-      </c>
+      <c r="A240" s="1"/>
+      <c r="B240" s="2"/>
     </row>
     <row r="241" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A241" s="1">
-        <v>239</v>
-      </c>
-      <c r="B241" s="2" t="str">
-        <f t="shared" si="14"/>
-        <v>/results/</v>
-      </c>
+      <c r="A241" s="1"/>
+      <c r="B241" s="2"/>
     </row>
     <row r="242" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A242" s="1">
-        <v>240</v>
-      </c>
-      <c r="B242" s="2" t="str">
-        <f t="shared" si="14"/>
-        <v>/results/</v>
-      </c>
+      <c r="A242" s="1"/>
+      <c r="B242" s="2"/>
     </row>
     <row r="243" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A243" s="1">
-        <v>241</v>
-      </c>
-      <c r="B243" s="2" t="str">
-        <f t="shared" si="14"/>
-        <v>/results/</v>
-      </c>
+      <c r="A243" s="1"/>
+      <c r="B243" s="2"/>
     </row>
     <row r="244" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A244" s="1">
-        <v>242</v>
-      </c>
-      <c r="B244" s="2" t="str">
-        <f t="shared" si="14"/>
-        <v>/results/</v>
-      </c>
+      <c r="A244" s="1"/>
+      <c r="B244" s="2"/>
     </row>
     <row r="245" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A245" s="1">
-        <v>243</v>
-      </c>
-      <c r="B245" s="2" t="str">
-        <f t="shared" si="14"/>
-        <v>/results/</v>
-      </c>
+      <c r="A245" s="1"/>
+      <c r="B245" s="2"/>
     </row>
     <row r="246" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A246" s="1">
-        <v>244</v>
-      </c>
-      <c r="B246" s="2" t="str">
-        <f t="shared" si="14"/>
-        <v>/results/</v>
-      </c>
+      <c r="A246" s="1"/>
+      <c r="B246" s="2"/>
     </row>
     <row r="247" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A247" s="1">
-        <v>245</v>
-      </c>
-      <c r="B247" s="2" t="str">
-        <f t="shared" si="14"/>
-        <v>/results/</v>
-      </c>
+      <c r="A247" s="1"/>
+      <c r="B247" s="2"/>
     </row>
     <row r="248" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A248" s="1">
-        <v>246</v>
-      </c>
-      <c r="B248" s="2" t="str">
-        <f t="shared" si="14"/>
-        <v>/results/</v>
-      </c>
+      <c r="A248" s="1"/>
+      <c r="B248" s="2"/>
     </row>
     <row r="249" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A249" s="1">
-        <v>247</v>
-      </c>
-      <c r="B249" s="2" t="str">
-        <f t="shared" si="14"/>
-        <v>/results/</v>
-      </c>
+      <c r="A249" s="1"/>
+      <c r="B249" s="2"/>
     </row>
     <row r="250" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A250" s="1">
-        <v>248</v>
-      </c>
-      <c r="B250" s="2" t="str">
-        <f t="shared" si="14"/>
-        <v>/results/</v>
-      </c>
+      <c r="A250" s="1"/>
+      <c r="B250" s="2"/>
     </row>
     <row r="251" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A251" s="1">
-        <v>249</v>
-      </c>
-      <c r="B251" s="2" t="str">
-        <f t="shared" si="14"/>
-        <v>/results/</v>
-      </c>
+      <c r="A251" s="1"/>
+      <c r="B251" s="2"/>
     </row>
     <row r="252" spans="1:2" x14ac:dyDescent="0.3">
-      <c r="A252" s="1">
-        <v>250</v>
-      </c>
-      <c r="B252" s="2" t="str">
-        <f t="shared" si="14"/>
-        <v>/results/</v>
-      </c>
+      <c r="A252" s="1"/>
+      <c r="B252" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="3" type="noConversion"/>
@@ -3408,19 +2453,17 @@
     <hyperlink ref="C21" r:id="rId17" xr:uid="{2A49AB25-C482-4B29-922B-9A7B04A5896C}"/>
     <hyperlink ref="B32" r:id="rId18" display="https://www.flashscore.com/football/albania/superliga-2019-2020/results/" xr:uid="{87CE32E0-0590-4132-86D3-255A5CF67D8C}"/>
     <hyperlink ref="B33:B41" r:id="rId19" display="https://www.flashscore.com/football/czech-republic/division-2" xr:uid="{01BB8C53-9909-451C-9206-4FA8274C88AB}"/>
-    <hyperlink ref="B62" r:id="rId20" display="https://www.flashscore.com/football/albania/superliga-2019-2020/results/" xr:uid="{1739D734-9899-449B-B559-B79E60FBE3E5}"/>
-    <hyperlink ref="C63:C71" r:id="rId21" display="https://www.flashscore.com/football/albania/superliga-" xr:uid="{21CCABB3-B02C-4EFC-BF95-EA408849CDD8}"/>
-    <hyperlink ref="B63:B71" r:id="rId22" display="https://www.flashscore.com/football/czech-republic/division-2" xr:uid="{577F8FD6-A1A1-48F0-91C4-E70027DF3C52}"/>
-    <hyperlink ref="C33" r:id="rId23" xr:uid="{9DB33A26-805E-4906-BB82-5353D125A597}"/>
-    <hyperlink ref="C35" r:id="rId24" xr:uid="{3144CFDE-2608-4294-9795-AD169319E10B}"/>
-    <hyperlink ref="C37" r:id="rId25" xr:uid="{72B7E17E-1D7B-4798-B1AB-C770EE9CE812}"/>
-    <hyperlink ref="C39" r:id="rId26" xr:uid="{3A8B6F78-1355-4FD9-AE69-99A272BD63CD}"/>
-    <hyperlink ref="C41" r:id="rId27" xr:uid="{DE8FFECE-0B99-4DAE-A17A-04C05E47F834}"/>
-    <hyperlink ref="C43" r:id="rId28" xr:uid="{FF2C6AC1-D9EB-4F07-8F9D-F2BBA4960974}"/>
-    <hyperlink ref="C45" r:id="rId29" xr:uid="{09D301E8-EF97-4707-97A8-8C00D81C51AA}"/>
-    <hyperlink ref="C47" r:id="rId30" xr:uid="{F7D8AFB2-300F-453B-B43C-F79E1E8B818C}"/>
-    <hyperlink ref="C49" r:id="rId31" xr:uid="{1901699E-371E-4820-BB0B-30E6A51BD797}"/>
-    <hyperlink ref="C51" r:id="rId32" xr:uid="{4EAC4529-F332-4F77-B53F-E54837943873}"/>
+    <hyperlink ref="C63:C71" r:id="rId20" display="https://www.flashscore.com/football/albania/superliga-" xr:uid="{21CCABB3-B02C-4EFC-BF95-EA408849CDD8}"/>
+    <hyperlink ref="C33" r:id="rId21" xr:uid="{9DB33A26-805E-4906-BB82-5353D125A597}"/>
+    <hyperlink ref="C35" r:id="rId22" xr:uid="{3144CFDE-2608-4294-9795-AD169319E10B}"/>
+    <hyperlink ref="C37" r:id="rId23" xr:uid="{72B7E17E-1D7B-4798-B1AB-C770EE9CE812}"/>
+    <hyperlink ref="C39" r:id="rId24" xr:uid="{3A8B6F78-1355-4FD9-AE69-99A272BD63CD}"/>
+    <hyperlink ref="C41" r:id="rId25" xr:uid="{DE8FFECE-0B99-4DAE-A17A-04C05E47F834}"/>
+    <hyperlink ref="C43" r:id="rId26" xr:uid="{FF2C6AC1-D9EB-4F07-8F9D-F2BBA4960974}"/>
+    <hyperlink ref="C45" r:id="rId27" xr:uid="{09D301E8-EF97-4707-97A8-8C00D81C51AA}"/>
+    <hyperlink ref="C47" r:id="rId28" xr:uid="{F7D8AFB2-300F-453B-B43C-F79E1E8B818C}"/>
+    <hyperlink ref="C49" r:id="rId29" xr:uid="{1901699E-371E-4820-BB0B-30E6A51BD797}"/>
+    <hyperlink ref="C51" r:id="rId30" xr:uid="{4EAC4529-F332-4F77-B53F-E54837943873}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>